<commit_message>
Fixed various things in the processor and simulation code; processor now at least executes nops and stop sanely.
</commit_message>
<xml_diff>
--- a/doc/rvex_pipeline_control.xlsx
+++ b/doc/rvex_pipeline_control.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="15240" windowHeight="7905"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="15240" windowHeight="7905" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LIMMH prefetch" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2337" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2338" uniqueCount="338">
   <si>
     <t>IF</t>
   </si>
@@ -1028,6 +1028,9 @@
   </si>
   <si>
     <t>Branch behavior with LIMMH from previous syllable enabled</t>
+  </si>
+  <si>
+    <t>exceptionPending is forwarded like the exception data, i.e. with one cycle delay. To get the first instruction of the trap handler to fetch, exceptionPending is overridden 0 when an exception is active.</t>
   </si>
 </sst>
 </file>
@@ -1888,7 +1891,13 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1900,22 +1909,19 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1927,16 +1933,19 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1948,19 +1957,13 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2488,7 +2491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:AM27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
@@ -3538,10 +3541,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:AK267"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5100" topLeftCell="A39" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="5100" topLeftCell="A4" activePane="bottomLeft"/>
       <selection activeCell="M12" sqref="M12:M13"/>
-      <selection pane="bottomLeft" activeCell="Q35" sqref="Q35"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3972,6 +3975,11 @@
     <row r="23" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C23" s="2" t="s">
         <v>284</v>
+      </c>
+    </row>
+    <row r="24" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C24" s="2" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="28" spans="3:20" ht="21" x14ac:dyDescent="0.35">
@@ -10023,7 +10031,7 @@
       <c r="D6" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="E6" s="170" t="s">
+      <c r="E6" s="172" t="s">
         <v>111</v>
       </c>
       <c r="F6" s="41" t="s">
@@ -10089,25 +10097,25 @@
       <c r="Z6" s="64" t="s">
         <v>109</v>
       </c>
-      <c r="AA6" s="177" t="s">
+      <c r="AA6" s="193" t="s">
         <v>108</v>
       </c>
-      <c r="AB6" s="177"/>
-      <c r="AC6" s="177"/>
-      <c r="AD6" s="177"/>
-      <c r="AE6" s="192" t="s">
+      <c r="AB6" s="193"/>
+      <c r="AC6" s="193"/>
+      <c r="AD6" s="193"/>
+      <c r="AE6" s="169" t="s">
         <v>89</v>
       </c>
-      <c r="AF6" s="192"/>
-      <c r="AG6" s="192"/>
+      <c r="AF6" s="169"/>
+      <c r="AG6" s="169"/>
       <c r="AH6" s="64" t="s">
         <v>107</v>
       </c>
-      <c r="AI6" s="173" t="s">
+      <c r="AI6" s="184" t="s">
         <v>54</v>
       </c>
-      <c r="AJ6" s="173"/>
-      <c r="AK6" s="173"/>
+      <c r="AJ6" s="184"/>
+      <c r="AK6" s="184"/>
       <c r="AL6" s="61" t="s">
         <v>52</v>
       </c>
@@ -10129,74 +10137,74 @@
         <f t="shared" ref="D7:D37" si="2">DEC2HEX(HEX2DEC(D6)+4)</f>
         <v>FFFFFF84</v>
       </c>
-      <c r="E7" s="171"/>
+      <c r="E7" s="173"/>
       <c r="F7" s="50" t="s">
         <v>106</v>
       </c>
       <c r="G7" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="H7" s="169" t="s">
+      <c r="H7" s="175" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="169"/>
-      <c r="J7" s="169"/>
+      <c r="I7" s="175"/>
+      <c r="J7" s="175"/>
       <c r="K7" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="L7" s="169" t="s">
+      <c r="L7" s="175" t="s">
         <v>61</v>
       </c>
-      <c r="M7" s="169"/>
-      <c r="N7" s="169"/>
+      <c r="M7" s="175"/>
+      <c r="N7" s="175"/>
       <c r="O7" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="P7" s="169" t="s">
+      <c r="P7" s="175" t="s">
         <v>62</v>
       </c>
-      <c r="Q7" s="169"/>
-      <c r="R7" s="169"/>
+      <c r="Q7" s="175"/>
+      <c r="R7" s="175"/>
       <c r="S7" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="T7" s="169" t="s">
+      <c r="T7" s="175" t="s">
         <v>63</v>
       </c>
-      <c r="U7" s="169"/>
-      <c r="V7" s="169"/>
+      <c r="U7" s="175"/>
+      <c r="V7" s="175"/>
       <c r="W7" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="X7" s="169" t="s">
+      <c r="X7" s="175" t="s">
         <v>56</v>
       </c>
-      <c r="Y7" s="169"/>
-      <c r="Z7" s="169"/>
+      <c r="Y7" s="175"/>
+      <c r="Z7" s="175"/>
       <c r="AA7" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="AB7" s="169" t="s">
+      <c r="AB7" s="175" t="s">
         <v>57</v>
       </c>
-      <c r="AC7" s="169"/>
-      <c r="AD7" s="169"/>
+      <c r="AC7" s="175"/>
+      <c r="AD7" s="175"/>
       <c r="AE7" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="AF7" s="169" t="s">
+      <c r="AF7" s="175" t="s">
         <v>58</v>
       </c>
-      <c r="AG7" s="169"/>
-      <c r="AH7" s="169"/>
+      <c r="AG7" s="175"/>
+      <c r="AH7" s="175"/>
       <c r="AI7" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="AJ7" s="169" t="s">
+      <c r="AJ7" s="175" t="s">
         <v>59</v>
       </c>
-      <c r="AK7" s="169"/>
-      <c r="AL7" s="174"/>
+      <c r="AK7" s="175"/>
+      <c r="AL7" s="192"/>
       <c r="AM7" s="2"/>
       <c r="AN7" s="2" t="s">
         <v>72</v>
@@ -10215,74 +10223,74 @@
         <f t="shared" si="2"/>
         <v>FFFFFF88</v>
       </c>
-      <c r="E8" s="171"/>
+      <c r="E8" s="173"/>
       <c r="F8" s="50" t="s">
         <v>104</v>
       </c>
       <c r="G8" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="H8" s="175" t="s">
+      <c r="H8" s="176" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="175"/>
-      <c r="J8" s="175"/>
+      <c r="I8" s="176"/>
+      <c r="J8" s="176"/>
       <c r="K8" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="L8" s="175" t="s">
+      <c r="L8" s="176" t="s">
         <v>61</v>
       </c>
-      <c r="M8" s="175"/>
-      <c r="N8" s="175"/>
+      <c r="M8" s="176"/>
+      <c r="N8" s="176"/>
       <c r="O8" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="P8" s="175" t="s">
+      <c r="P8" s="176" t="s">
         <v>62</v>
       </c>
-      <c r="Q8" s="175"/>
-      <c r="R8" s="175"/>
+      <c r="Q8" s="176"/>
+      <c r="R8" s="176"/>
       <c r="S8" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="T8" s="175" t="s">
+      <c r="T8" s="176" t="s">
         <v>63</v>
       </c>
-      <c r="U8" s="175"/>
-      <c r="V8" s="175"/>
+      <c r="U8" s="176"/>
+      <c r="V8" s="176"/>
       <c r="W8" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="X8" s="175" t="s">
+      <c r="X8" s="176" t="s">
         <v>56</v>
       </c>
-      <c r="Y8" s="175"/>
-      <c r="Z8" s="175"/>
+      <c r="Y8" s="176"/>
+      <c r="Z8" s="176"/>
       <c r="AA8" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="AB8" s="175" t="s">
+      <c r="AB8" s="176" t="s">
         <v>57</v>
       </c>
-      <c r="AC8" s="175"/>
-      <c r="AD8" s="175"/>
+      <c r="AC8" s="176"/>
+      <c r="AD8" s="176"/>
       <c r="AE8" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="AF8" s="175" t="s">
+      <c r="AF8" s="176" t="s">
         <v>58</v>
       </c>
-      <c r="AG8" s="175"/>
-      <c r="AH8" s="175"/>
+      <c r="AG8" s="176"/>
+      <c r="AH8" s="176"/>
       <c r="AI8" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="AJ8" s="175" t="s">
+      <c r="AJ8" s="176" t="s">
         <v>59</v>
       </c>
-      <c r="AK8" s="175"/>
-      <c r="AL8" s="176"/>
+      <c r="AK8" s="176"/>
+      <c r="AL8" s="191"/>
       <c r="AM8" s="2"/>
       <c r="AN8" s="2" t="s">
         <v>72</v>
@@ -10301,74 +10309,74 @@
         <f t="shared" si="2"/>
         <v>FFFFFF8C</v>
       </c>
-      <c r="E9" s="171"/>
+      <c r="E9" s="173"/>
       <c r="F9" s="50" t="s">
         <v>105</v>
       </c>
       <c r="G9" s="48">
         <v>0</v>
       </c>
-      <c r="H9" s="175" t="s">
+      <c r="H9" s="176" t="s">
         <v>79</v>
       </c>
-      <c r="I9" s="175"/>
-      <c r="J9" s="175"/>
+      <c r="I9" s="176"/>
+      <c r="J9" s="176"/>
       <c r="K9" s="32">
         <v>0</v>
       </c>
-      <c r="L9" s="175" t="s">
+      <c r="L9" s="176" t="s">
         <v>80</v>
       </c>
-      <c r="M9" s="175"/>
-      <c r="N9" s="175"/>
+      <c r="M9" s="176"/>
+      <c r="N9" s="176"/>
       <c r="O9" s="32">
         <v>0</v>
       </c>
-      <c r="P9" s="175" t="s">
+      <c r="P9" s="176" t="s">
         <v>81</v>
       </c>
-      <c r="Q9" s="175"/>
-      <c r="R9" s="175"/>
+      <c r="Q9" s="176"/>
+      <c r="R9" s="176"/>
       <c r="S9" s="32">
         <v>0</v>
       </c>
-      <c r="T9" s="175" t="s">
+      <c r="T9" s="176" t="s">
         <v>82</v>
       </c>
-      <c r="U9" s="175"/>
-      <c r="V9" s="175"/>
+      <c r="U9" s="176"/>
+      <c r="V9" s="176"/>
       <c r="W9" s="32">
         <v>0</v>
       </c>
-      <c r="X9" s="175" t="s">
+      <c r="X9" s="176" t="s">
         <v>83</v>
       </c>
-      <c r="Y9" s="175"/>
-      <c r="Z9" s="175"/>
+      <c r="Y9" s="176"/>
+      <c r="Z9" s="176"/>
       <c r="AA9" s="32">
         <v>0</v>
       </c>
-      <c r="AB9" s="175" t="s">
+      <c r="AB9" s="176" t="s">
         <v>84</v>
       </c>
-      <c r="AC9" s="175"/>
-      <c r="AD9" s="175"/>
+      <c r="AC9" s="176"/>
+      <c r="AD9" s="176"/>
       <c r="AE9" s="32">
         <v>0</v>
       </c>
-      <c r="AF9" s="175" t="s">
+      <c r="AF9" s="176" t="s">
         <v>85</v>
       </c>
-      <c r="AG9" s="175"/>
-      <c r="AH9" s="175"/>
+      <c r="AG9" s="176"/>
+      <c r="AH9" s="176"/>
       <c r="AI9" s="32">
         <v>0</v>
       </c>
-      <c r="AJ9" s="175" t="s">
+      <c r="AJ9" s="176" t="s">
         <v>86</v>
       </c>
-      <c r="AK9" s="175"/>
-      <c r="AL9" s="176"/>
+      <c r="AK9" s="176"/>
+      <c r="AL9" s="191"/>
       <c r="AM9" s="2"/>
       <c r="AN9" s="2" t="s">
         <v>87</v>
@@ -10387,7 +10395,7 @@
         <f t="shared" si="2"/>
         <v>FFFFFF90</v>
       </c>
-      <c r="E10" s="171"/>
+      <c r="E10" s="173"/>
       <c r="F10" s="47" t="s">
         <v>51</v>
       </c>
@@ -10503,7 +10511,7 @@
         <f t="shared" si="2"/>
         <v>FFFFFF94</v>
       </c>
-      <c r="E11" s="171"/>
+      <c r="E11" s="173"/>
       <c r="F11" s="47" t="s">
         <v>51</v>
       </c>
@@ -10619,7 +10627,7 @@
         <f t="shared" si="2"/>
         <v>FFFFFF98</v>
       </c>
-      <c r="E12" s="171"/>
+      <c r="E12" s="173"/>
       <c r="F12" s="47" t="s">
         <v>51</v>
       </c>
@@ -10735,7 +10743,7 @@
         <f t="shared" si="2"/>
         <v>FFFFFF9C</v>
       </c>
-      <c r="E13" s="172"/>
+      <c r="E13" s="174"/>
       <c r="F13" s="50" t="s">
         <v>113</v>
       </c>
@@ -10853,7 +10861,7 @@
         <f t="shared" si="2"/>
         <v>FFFFFFA0</v>
       </c>
-      <c r="E14" s="170" t="s">
+      <c r="E14" s="172" t="s">
         <v>122</v>
       </c>
       <c r="F14" s="41" t="s">
@@ -10975,44 +10983,44 @@
         <f t="shared" si="2"/>
         <v>FFFFFFA4</v>
       </c>
-      <c r="E15" s="171"/>
+      <c r="E15" s="173"/>
       <c r="F15" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="G15" s="179" t="s">
+      <c r="G15" s="180" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="180"/>
-      <c r="I15" s="180"/>
-      <c r="J15" s="180"/>
-      <c r="K15" s="180"/>
-      <c r="L15" s="180"/>
-      <c r="M15" s="180"/>
-      <c r="N15" s="180"/>
-      <c r="O15" s="180"/>
-      <c r="P15" s="180"/>
-      <c r="Q15" s="180"/>
-      <c r="R15" s="180"/>
-      <c r="S15" s="180"/>
-      <c r="T15" s="180"/>
-      <c r="U15" s="180"/>
-      <c r="V15" s="180"/>
-      <c r="W15" s="180"/>
-      <c r="X15" s="180"/>
-      <c r="Y15" s="180"/>
-      <c r="Z15" s="180"/>
-      <c r="AA15" s="180"/>
-      <c r="AB15" s="180"/>
-      <c r="AC15" s="180"/>
-      <c r="AD15" s="180"/>
-      <c r="AE15" s="180"/>
-      <c r="AF15" s="180"/>
-      <c r="AG15" s="180"/>
-      <c r="AH15" s="180"/>
-      <c r="AI15" s="180"/>
-      <c r="AJ15" s="180"/>
-      <c r="AK15" s="180"/>
-      <c r="AL15" s="181"/>
+      <c r="H15" s="181"/>
+      <c r="I15" s="181"/>
+      <c r="J15" s="181"/>
+      <c r="K15" s="181"/>
+      <c r="L15" s="181"/>
+      <c r="M15" s="181"/>
+      <c r="N15" s="181"/>
+      <c r="O15" s="181"/>
+      <c r="P15" s="181"/>
+      <c r="Q15" s="181"/>
+      <c r="R15" s="181"/>
+      <c r="S15" s="181"/>
+      <c r="T15" s="181"/>
+      <c r="U15" s="181"/>
+      <c r="V15" s="181"/>
+      <c r="W15" s="181"/>
+      <c r="X15" s="181"/>
+      <c r="Y15" s="181"/>
+      <c r="Z15" s="181"/>
+      <c r="AA15" s="181"/>
+      <c r="AB15" s="181"/>
+      <c r="AC15" s="181"/>
+      <c r="AD15" s="181"/>
+      <c r="AE15" s="181"/>
+      <c r="AF15" s="181"/>
+      <c r="AG15" s="181"/>
+      <c r="AH15" s="181"/>
+      <c r="AI15" s="181"/>
+      <c r="AJ15" s="181"/>
+      <c r="AK15" s="181"/>
+      <c r="AL15" s="182"/>
       <c r="AM15" s="2"/>
       <c r="AN15" s="2" t="s">
         <v>37</v>
@@ -11031,44 +11039,44 @@
         <f t="shared" si="2"/>
         <v>FFFFFFA8</v>
       </c>
-      <c r="E16" s="171"/>
+      <c r="E16" s="173"/>
       <c r="F16" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="G16" s="179" t="s">
+      <c r="G16" s="180" t="s">
         <v>98</v>
       </c>
-      <c r="H16" s="180"/>
-      <c r="I16" s="180"/>
-      <c r="J16" s="180"/>
-      <c r="K16" s="180"/>
-      <c r="L16" s="180"/>
-      <c r="M16" s="180"/>
-      <c r="N16" s="180"/>
-      <c r="O16" s="180"/>
-      <c r="P16" s="180"/>
-      <c r="Q16" s="180"/>
-      <c r="R16" s="180"/>
-      <c r="S16" s="180"/>
-      <c r="T16" s="180"/>
-      <c r="U16" s="180"/>
-      <c r="V16" s="180"/>
-      <c r="W16" s="180"/>
-      <c r="X16" s="180"/>
-      <c r="Y16" s="180"/>
-      <c r="Z16" s="180"/>
-      <c r="AA16" s="180"/>
-      <c r="AB16" s="180"/>
-      <c r="AC16" s="180"/>
-      <c r="AD16" s="180"/>
-      <c r="AE16" s="180"/>
-      <c r="AF16" s="180"/>
-      <c r="AG16" s="180"/>
-      <c r="AH16" s="180"/>
-      <c r="AI16" s="180"/>
-      <c r="AJ16" s="180"/>
-      <c r="AK16" s="180"/>
-      <c r="AL16" s="181"/>
+      <c r="H16" s="181"/>
+      <c r="I16" s="181"/>
+      <c r="J16" s="181"/>
+      <c r="K16" s="181"/>
+      <c r="L16" s="181"/>
+      <c r="M16" s="181"/>
+      <c r="N16" s="181"/>
+      <c r="O16" s="181"/>
+      <c r="P16" s="181"/>
+      <c r="Q16" s="181"/>
+      <c r="R16" s="181"/>
+      <c r="S16" s="181"/>
+      <c r="T16" s="181"/>
+      <c r="U16" s="181"/>
+      <c r="V16" s="181"/>
+      <c r="W16" s="181"/>
+      <c r="X16" s="181"/>
+      <c r="Y16" s="181"/>
+      <c r="Z16" s="181"/>
+      <c r="AA16" s="181"/>
+      <c r="AB16" s="181"/>
+      <c r="AC16" s="181"/>
+      <c r="AD16" s="181"/>
+      <c r="AE16" s="181"/>
+      <c r="AF16" s="181"/>
+      <c r="AG16" s="181"/>
+      <c r="AH16" s="181"/>
+      <c r="AI16" s="181"/>
+      <c r="AJ16" s="181"/>
+      <c r="AK16" s="181"/>
+      <c r="AL16" s="182"/>
       <c r="AM16" s="2"/>
       <c r="AN16" s="2" t="s">
         <v>112</v>
@@ -11087,7 +11095,7 @@
         <f t="shared" si="2"/>
         <v>FFFFFFAC</v>
       </c>
-      <c r="E17" s="171"/>
+      <c r="E17" s="173"/>
       <c r="F17" s="50" t="s">
         <v>125</v>
       </c>
@@ -11205,7 +11213,7 @@
         <f t="shared" si="2"/>
         <v>FFFFFFB0</v>
       </c>
-      <c r="E18" s="171"/>
+      <c r="E18" s="173"/>
       <c r="F18" s="76" t="s">
         <v>26</v>
       </c>
@@ -11281,16 +11289,16 @@
       <c r="AD18" s="32">
         <v>0</v>
       </c>
-      <c r="AE18" s="180" t="s">
+      <c r="AE18" s="181" t="s">
         <v>27</v>
       </c>
-      <c r="AF18" s="180"/>
-      <c r="AG18" s="180"/>
-      <c r="AH18" s="180"/>
-      <c r="AI18" s="180"/>
-      <c r="AJ18" s="180"/>
-      <c r="AK18" s="180"/>
-      <c r="AL18" s="181"/>
+      <c r="AF18" s="181"/>
+      <c r="AG18" s="181"/>
+      <c r="AH18" s="181"/>
+      <c r="AI18" s="181"/>
+      <c r="AJ18" s="181"/>
+      <c r="AK18" s="181"/>
+      <c r="AL18" s="182"/>
       <c r="AM18" s="2"/>
       <c r="AN18" s="2" t="s">
         <v>28</v>
@@ -11309,44 +11317,44 @@
         <f t="shared" si="2"/>
         <v>FFFFFFB4</v>
       </c>
-      <c r="E19" s="171"/>
+      <c r="E19" s="173"/>
       <c r="F19" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="179" t="s">
+      <c r="G19" s="180" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="180"/>
-      <c r="I19" s="180"/>
-      <c r="J19" s="180"/>
-      <c r="K19" s="180"/>
-      <c r="L19" s="180"/>
-      <c r="M19" s="180"/>
-      <c r="N19" s="180"/>
-      <c r="O19" s="180"/>
-      <c r="P19" s="180"/>
-      <c r="Q19" s="180"/>
-      <c r="R19" s="180"/>
-      <c r="S19" s="180"/>
-      <c r="T19" s="180"/>
-      <c r="U19" s="180"/>
-      <c r="V19" s="180"/>
-      <c r="W19" s="180"/>
-      <c r="X19" s="180"/>
-      <c r="Y19" s="180"/>
-      <c r="Z19" s="180"/>
-      <c r="AA19" s="180"/>
-      <c r="AB19" s="180"/>
-      <c r="AC19" s="180"/>
-      <c r="AD19" s="180"/>
-      <c r="AE19" s="180"/>
-      <c r="AF19" s="180"/>
-      <c r="AG19" s="180"/>
-      <c r="AH19" s="180"/>
-      <c r="AI19" s="180"/>
-      <c r="AJ19" s="180"/>
-      <c r="AK19" s="180"/>
-      <c r="AL19" s="181"/>
+      <c r="H19" s="181"/>
+      <c r="I19" s="181"/>
+      <c r="J19" s="181"/>
+      <c r="K19" s="181"/>
+      <c r="L19" s="181"/>
+      <c r="M19" s="181"/>
+      <c r="N19" s="181"/>
+      <c r="O19" s="181"/>
+      <c r="P19" s="181"/>
+      <c r="Q19" s="181"/>
+      <c r="R19" s="181"/>
+      <c r="S19" s="181"/>
+      <c r="T19" s="181"/>
+      <c r="U19" s="181"/>
+      <c r="V19" s="181"/>
+      <c r="W19" s="181"/>
+      <c r="X19" s="181"/>
+      <c r="Y19" s="181"/>
+      <c r="Z19" s="181"/>
+      <c r="AA19" s="181"/>
+      <c r="AB19" s="181"/>
+      <c r="AC19" s="181"/>
+      <c r="AD19" s="181"/>
+      <c r="AE19" s="181"/>
+      <c r="AF19" s="181"/>
+      <c r="AG19" s="181"/>
+      <c r="AH19" s="181"/>
+      <c r="AI19" s="181"/>
+      <c r="AJ19" s="181"/>
+      <c r="AK19" s="181"/>
+      <c r="AL19" s="182"/>
       <c r="AM19" s="2"/>
       <c r="AN19" s="2" t="s">
         <v>29</v>
@@ -11365,44 +11373,44 @@
         <f t="shared" si="2"/>
         <v>FFFFFFB8</v>
       </c>
-      <c r="E20" s="171"/>
+      <c r="E20" s="173"/>
       <c r="F20" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="185" t="s">
+      <c r="G20" s="186" t="s">
         <v>30</v>
       </c>
-      <c r="H20" s="178"/>
-      <c r="I20" s="178"/>
-      <c r="J20" s="178"/>
-      <c r="K20" s="178"/>
-      <c r="L20" s="178"/>
-      <c r="M20" s="178"/>
-      <c r="N20" s="178"/>
-      <c r="O20" s="178"/>
-      <c r="P20" s="178"/>
-      <c r="Q20" s="178"/>
-      <c r="R20" s="178"/>
-      <c r="S20" s="178"/>
-      <c r="T20" s="178"/>
-      <c r="U20" s="178"/>
-      <c r="V20" s="178"/>
-      <c r="W20" s="178"/>
-      <c r="X20" s="178"/>
-      <c r="Y20" s="178"/>
-      <c r="Z20" s="178"/>
-      <c r="AA20" s="178"/>
-      <c r="AB20" s="178"/>
-      <c r="AC20" s="178"/>
-      <c r="AD20" s="178"/>
-      <c r="AE20" s="178"/>
-      <c r="AF20" s="178"/>
-      <c r="AG20" s="178"/>
-      <c r="AH20" s="178"/>
-      <c r="AI20" s="178"/>
-      <c r="AJ20" s="178"/>
-      <c r="AK20" s="178"/>
-      <c r="AL20" s="186"/>
+      <c r="H20" s="187"/>
+      <c r="I20" s="187"/>
+      <c r="J20" s="187"/>
+      <c r="K20" s="187"/>
+      <c r="L20" s="187"/>
+      <c r="M20" s="187"/>
+      <c r="N20" s="187"/>
+      <c r="O20" s="187"/>
+      <c r="P20" s="187"/>
+      <c r="Q20" s="187"/>
+      <c r="R20" s="187"/>
+      <c r="S20" s="187"/>
+      <c r="T20" s="187"/>
+      <c r="U20" s="187"/>
+      <c r="V20" s="187"/>
+      <c r="W20" s="187"/>
+      <c r="X20" s="187"/>
+      <c r="Y20" s="187"/>
+      <c r="Z20" s="187"/>
+      <c r="AA20" s="187"/>
+      <c r="AB20" s="187"/>
+      <c r="AC20" s="187"/>
+      <c r="AD20" s="187"/>
+      <c r="AE20" s="187"/>
+      <c r="AF20" s="187"/>
+      <c r="AG20" s="187"/>
+      <c r="AH20" s="187"/>
+      <c r="AI20" s="187"/>
+      <c r="AJ20" s="187"/>
+      <c r="AK20" s="187"/>
+      <c r="AL20" s="188"/>
       <c r="AM20" s="2"/>
       <c r="AN20" s="2" t="s">
         <v>31</v>
@@ -11421,7 +11429,7 @@
         <f t="shared" si="2"/>
         <v>FFFFFFBC</v>
       </c>
-      <c r="E21" s="171"/>
+      <c r="E21" s="173"/>
       <c r="F21" s="76" t="s">
         <v>12</v>
       </c>
@@ -11539,44 +11547,44 @@
         <f t="shared" si="2"/>
         <v>FFFFFFC0</v>
       </c>
-      <c r="E22" s="171"/>
+      <c r="E22" s="173"/>
       <c r="F22" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="G22" s="185" t="s">
+      <c r="G22" s="186" t="s">
         <v>75</v>
       </c>
-      <c r="H22" s="178"/>
-      <c r="I22" s="178"/>
-      <c r="J22" s="178"/>
-      <c r="K22" s="178"/>
-      <c r="L22" s="178"/>
-      <c r="M22" s="178"/>
-      <c r="N22" s="178"/>
-      <c r="O22" s="178"/>
-      <c r="P22" s="178"/>
-      <c r="Q22" s="178"/>
-      <c r="R22" s="178"/>
-      <c r="S22" s="178"/>
-      <c r="T22" s="178"/>
-      <c r="U22" s="178"/>
-      <c r="V22" s="178"/>
-      <c r="W22" s="178"/>
-      <c r="X22" s="178"/>
-      <c r="Y22" s="178"/>
-      <c r="Z22" s="178"/>
-      <c r="AA22" s="178"/>
-      <c r="AB22" s="178"/>
-      <c r="AC22" s="178"/>
-      <c r="AD22" s="178"/>
-      <c r="AE22" s="178"/>
-      <c r="AF22" s="178"/>
-      <c r="AG22" s="178"/>
-      <c r="AH22" s="178"/>
-      <c r="AI22" s="178"/>
-      <c r="AJ22" s="178"/>
-      <c r="AK22" s="178"/>
-      <c r="AL22" s="186"/>
+      <c r="H22" s="187"/>
+      <c r="I22" s="187"/>
+      <c r="J22" s="187"/>
+      <c r="K22" s="187"/>
+      <c r="L22" s="187"/>
+      <c r="M22" s="187"/>
+      <c r="N22" s="187"/>
+      <c r="O22" s="187"/>
+      <c r="P22" s="187"/>
+      <c r="Q22" s="187"/>
+      <c r="R22" s="187"/>
+      <c r="S22" s="187"/>
+      <c r="T22" s="187"/>
+      <c r="U22" s="187"/>
+      <c r="V22" s="187"/>
+      <c r="W22" s="187"/>
+      <c r="X22" s="187"/>
+      <c r="Y22" s="187"/>
+      <c r="Z22" s="187"/>
+      <c r="AA22" s="187"/>
+      <c r="AB22" s="187"/>
+      <c r="AC22" s="187"/>
+      <c r="AD22" s="187"/>
+      <c r="AE22" s="187"/>
+      <c r="AF22" s="187"/>
+      <c r="AG22" s="187"/>
+      <c r="AH22" s="187"/>
+      <c r="AI22" s="187"/>
+      <c r="AJ22" s="187"/>
+      <c r="AK22" s="187"/>
+      <c r="AL22" s="188"/>
       <c r="AM22" s="2"/>
       <c r="AN22" s="2" t="s">
         <v>77</v>
@@ -11595,44 +11603,44 @@
         <f t="shared" si="2"/>
         <v>FFFFFFC4</v>
       </c>
-      <c r="E23" s="171"/>
+      <c r="E23" s="173"/>
       <c r="F23" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="G23" s="185" t="s">
+      <c r="G23" s="186" t="s">
         <v>76</v>
       </c>
-      <c r="H23" s="178"/>
-      <c r="I23" s="178"/>
-      <c r="J23" s="178"/>
-      <c r="K23" s="178"/>
-      <c r="L23" s="178"/>
-      <c r="M23" s="178"/>
-      <c r="N23" s="178"/>
-      <c r="O23" s="178"/>
-      <c r="P23" s="178"/>
-      <c r="Q23" s="178"/>
-      <c r="R23" s="178"/>
-      <c r="S23" s="178"/>
-      <c r="T23" s="178"/>
-      <c r="U23" s="178"/>
-      <c r="V23" s="178"/>
-      <c r="W23" s="178"/>
-      <c r="X23" s="178"/>
-      <c r="Y23" s="178"/>
-      <c r="Z23" s="178"/>
-      <c r="AA23" s="178"/>
-      <c r="AB23" s="178"/>
-      <c r="AC23" s="178"/>
-      <c r="AD23" s="178"/>
-      <c r="AE23" s="178"/>
-      <c r="AF23" s="178"/>
-      <c r="AG23" s="178"/>
-      <c r="AH23" s="178"/>
-      <c r="AI23" s="178"/>
-      <c r="AJ23" s="178"/>
-      <c r="AK23" s="178"/>
-      <c r="AL23" s="186"/>
+      <c r="H23" s="187"/>
+      <c r="I23" s="187"/>
+      <c r="J23" s="187"/>
+      <c r="K23" s="187"/>
+      <c r="L23" s="187"/>
+      <c r="M23" s="187"/>
+      <c r="N23" s="187"/>
+      <c r="O23" s="187"/>
+      <c r="P23" s="187"/>
+      <c r="Q23" s="187"/>
+      <c r="R23" s="187"/>
+      <c r="S23" s="187"/>
+      <c r="T23" s="187"/>
+      <c r="U23" s="187"/>
+      <c r="V23" s="187"/>
+      <c r="W23" s="187"/>
+      <c r="X23" s="187"/>
+      <c r="Y23" s="187"/>
+      <c r="Z23" s="187"/>
+      <c r="AA23" s="187"/>
+      <c r="AB23" s="187"/>
+      <c r="AC23" s="187"/>
+      <c r="AD23" s="187"/>
+      <c r="AE23" s="187"/>
+      <c r="AF23" s="187"/>
+      <c r="AG23" s="187"/>
+      <c r="AH23" s="187"/>
+      <c r="AI23" s="187"/>
+      <c r="AJ23" s="187"/>
+      <c r="AK23" s="187"/>
+      <c r="AL23" s="188"/>
       <c r="AM23" s="2"/>
       <c r="AN23" s="2" t="s">
         <v>78</v>
@@ -11651,7 +11659,7 @@
         <f t="shared" si="2"/>
         <v>FFFFFFC8</v>
       </c>
-      <c r="E24" s="171"/>
+      <c r="E24" s="173"/>
       <c r="F24" s="47" t="s">
         <v>51</v>
       </c>
@@ -11765,7 +11773,7 @@
         <f t="shared" si="2"/>
         <v>FFFFFFCC</v>
       </c>
-      <c r="E25" s="171"/>
+      <c r="E25" s="173"/>
       <c r="F25" s="47" t="s">
         <v>51</v>
       </c>
@@ -11880,44 +11888,44 @@
         <f t="shared" si="2"/>
         <v>FFFFFFD0</v>
       </c>
-      <c r="E26" s="171"/>
+      <c r="E26" s="173"/>
       <c r="F26" s="76" t="s">
         <v>100</v>
       </c>
-      <c r="G26" s="185" t="s">
+      <c r="G26" s="186" t="s">
         <v>32</v>
       </c>
-      <c r="H26" s="178"/>
-      <c r="I26" s="178"/>
-      <c r="J26" s="178"/>
-      <c r="K26" s="178"/>
-      <c r="L26" s="178"/>
-      <c r="M26" s="178"/>
-      <c r="N26" s="178"/>
-      <c r="O26" s="178"/>
-      <c r="P26" s="178"/>
-      <c r="Q26" s="178"/>
-      <c r="R26" s="178"/>
-      <c r="S26" s="178"/>
-      <c r="T26" s="178"/>
-      <c r="U26" s="178"/>
-      <c r="V26" s="178"/>
-      <c r="W26" s="178"/>
-      <c r="X26" s="178"/>
-      <c r="Y26" s="178"/>
-      <c r="Z26" s="178"/>
-      <c r="AA26" s="178"/>
-      <c r="AB26" s="178"/>
-      <c r="AC26" s="178"/>
-      <c r="AD26" s="178"/>
-      <c r="AE26" s="178"/>
-      <c r="AF26" s="178"/>
-      <c r="AG26" s="178"/>
-      <c r="AH26" s="178"/>
-      <c r="AI26" s="178"/>
-      <c r="AJ26" s="178"/>
-      <c r="AK26" s="178"/>
-      <c r="AL26" s="186"/>
+      <c r="H26" s="187"/>
+      <c r="I26" s="187"/>
+      <c r="J26" s="187"/>
+      <c r="K26" s="187"/>
+      <c r="L26" s="187"/>
+      <c r="M26" s="187"/>
+      <c r="N26" s="187"/>
+      <c r="O26" s="187"/>
+      <c r="P26" s="187"/>
+      <c r="Q26" s="187"/>
+      <c r="R26" s="187"/>
+      <c r="S26" s="187"/>
+      <c r="T26" s="187"/>
+      <c r="U26" s="187"/>
+      <c r="V26" s="187"/>
+      <c r="W26" s="187"/>
+      <c r="X26" s="187"/>
+      <c r="Y26" s="187"/>
+      <c r="Z26" s="187"/>
+      <c r="AA26" s="187"/>
+      <c r="AB26" s="187"/>
+      <c r="AC26" s="187"/>
+      <c r="AD26" s="187"/>
+      <c r="AE26" s="187"/>
+      <c r="AF26" s="187"/>
+      <c r="AG26" s="187"/>
+      <c r="AH26" s="187"/>
+      <c r="AI26" s="187"/>
+      <c r="AJ26" s="187"/>
+      <c r="AK26" s="187"/>
+      <c r="AL26" s="188"/>
       <c r="AM26" s="2"/>
       <c r="AN26" s="2" t="s">
         <v>38</v>
@@ -11936,44 +11944,44 @@
         <f t="shared" si="2"/>
         <v>FFFFFFD4</v>
       </c>
-      <c r="E27" s="171"/>
+      <c r="E27" s="173"/>
       <c r="F27" s="76" t="s">
         <v>101</v>
       </c>
-      <c r="G27" s="178" t="s">
+      <c r="G27" s="187" t="s">
         <v>33</v>
       </c>
-      <c r="H27" s="178"/>
-      <c r="I27" s="178"/>
-      <c r="J27" s="178"/>
-      <c r="K27" s="178"/>
-      <c r="L27" s="178"/>
-      <c r="M27" s="178"/>
-      <c r="N27" s="178"/>
-      <c r="O27" s="178"/>
-      <c r="P27" s="178"/>
-      <c r="Q27" s="178"/>
-      <c r="R27" s="178"/>
-      <c r="S27" s="178"/>
-      <c r="T27" s="178"/>
-      <c r="U27" s="178"/>
-      <c r="V27" s="178"/>
-      <c r="W27" s="178"/>
-      <c r="X27" s="178"/>
-      <c r="Y27" s="178"/>
-      <c r="Z27" s="178"/>
-      <c r="AA27" s="178"/>
-      <c r="AB27" s="178"/>
-      <c r="AC27" s="178"/>
-      <c r="AD27" s="178"/>
-      <c r="AE27" s="178"/>
-      <c r="AF27" s="178"/>
-      <c r="AG27" s="178"/>
-      <c r="AH27" s="178"/>
-      <c r="AI27" s="178"/>
-      <c r="AJ27" s="178"/>
-      <c r="AK27" s="178"/>
-      <c r="AL27" s="186"/>
+      <c r="H27" s="187"/>
+      <c r="I27" s="187"/>
+      <c r="J27" s="187"/>
+      <c r="K27" s="187"/>
+      <c r="L27" s="187"/>
+      <c r="M27" s="187"/>
+      <c r="N27" s="187"/>
+      <c r="O27" s="187"/>
+      <c r="P27" s="187"/>
+      <c r="Q27" s="187"/>
+      <c r="R27" s="187"/>
+      <c r="S27" s="187"/>
+      <c r="T27" s="187"/>
+      <c r="U27" s="187"/>
+      <c r="V27" s="187"/>
+      <c r="W27" s="187"/>
+      <c r="X27" s="187"/>
+      <c r="Y27" s="187"/>
+      <c r="Z27" s="187"/>
+      <c r="AA27" s="187"/>
+      <c r="AB27" s="187"/>
+      <c r="AC27" s="187"/>
+      <c r="AD27" s="187"/>
+      <c r="AE27" s="187"/>
+      <c r="AF27" s="187"/>
+      <c r="AG27" s="187"/>
+      <c r="AH27" s="187"/>
+      <c r="AI27" s="187"/>
+      <c r="AJ27" s="187"/>
+      <c r="AK27" s="187"/>
+      <c r="AL27" s="188"/>
       <c r="AM27" s="2"/>
       <c r="AN27" s="2" t="s">
         <v>41</v>
@@ -11992,44 +12000,44 @@
         <f t="shared" si="2"/>
         <v>FFFFFFD8</v>
       </c>
-      <c r="E28" s="171"/>
+      <c r="E28" s="173"/>
       <c r="F28" s="76" t="s">
         <v>102</v>
       </c>
-      <c r="G28" s="178" t="s">
+      <c r="G28" s="187" t="s">
         <v>34</v>
       </c>
-      <c r="H28" s="178"/>
-      <c r="I28" s="178"/>
-      <c r="J28" s="178"/>
-      <c r="K28" s="178"/>
-      <c r="L28" s="178"/>
-      <c r="M28" s="178"/>
-      <c r="N28" s="178"/>
-      <c r="O28" s="178"/>
-      <c r="P28" s="178"/>
-      <c r="Q28" s="178"/>
-      <c r="R28" s="178"/>
-      <c r="S28" s="178"/>
-      <c r="T28" s="178"/>
-      <c r="U28" s="178"/>
-      <c r="V28" s="178"/>
-      <c r="W28" s="178"/>
-      <c r="X28" s="178"/>
-      <c r="Y28" s="178"/>
-      <c r="Z28" s="178"/>
-      <c r="AA28" s="178"/>
-      <c r="AB28" s="178"/>
-      <c r="AC28" s="178"/>
-      <c r="AD28" s="178"/>
-      <c r="AE28" s="178"/>
-      <c r="AF28" s="178"/>
-      <c r="AG28" s="178"/>
-      <c r="AH28" s="178"/>
-      <c r="AI28" s="178"/>
-      <c r="AJ28" s="178"/>
-      <c r="AK28" s="178"/>
-      <c r="AL28" s="186"/>
+      <c r="H28" s="187"/>
+      <c r="I28" s="187"/>
+      <c r="J28" s="187"/>
+      <c r="K28" s="187"/>
+      <c r="L28" s="187"/>
+      <c r="M28" s="187"/>
+      <c r="N28" s="187"/>
+      <c r="O28" s="187"/>
+      <c r="P28" s="187"/>
+      <c r="Q28" s="187"/>
+      <c r="R28" s="187"/>
+      <c r="S28" s="187"/>
+      <c r="T28" s="187"/>
+      <c r="U28" s="187"/>
+      <c r="V28" s="187"/>
+      <c r="W28" s="187"/>
+      <c r="X28" s="187"/>
+      <c r="Y28" s="187"/>
+      <c r="Z28" s="187"/>
+      <c r="AA28" s="187"/>
+      <c r="AB28" s="187"/>
+      <c r="AC28" s="187"/>
+      <c r="AD28" s="187"/>
+      <c r="AE28" s="187"/>
+      <c r="AF28" s="187"/>
+      <c r="AG28" s="187"/>
+      <c r="AH28" s="187"/>
+      <c r="AI28" s="187"/>
+      <c r="AJ28" s="187"/>
+      <c r="AK28" s="187"/>
+      <c r="AL28" s="188"/>
       <c r="AM28" s="2"/>
       <c r="AN28" s="2" t="s">
         <v>40</v>
@@ -12048,44 +12056,44 @@
         <f t="shared" si="2"/>
         <v>FFFFFFDC</v>
       </c>
-      <c r="E29" s="171"/>
+      <c r="E29" s="173"/>
       <c r="F29" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="G29" s="185" t="s">
+      <c r="G29" s="186" t="s">
         <v>35</v>
       </c>
-      <c r="H29" s="178"/>
-      <c r="I29" s="178"/>
-      <c r="J29" s="178"/>
-      <c r="K29" s="178"/>
-      <c r="L29" s="178"/>
-      <c r="M29" s="178"/>
-      <c r="N29" s="178"/>
-      <c r="O29" s="178"/>
-      <c r="P29" s="178"/>
-      <c r="Q29" s="178"/>
-      <c r="R29" s="178"/>
-      <c r="S29" s="178"/>
-      <c r="T29" s="178"/>
-      <c r="U29" s="178"/>
-      <c r="V29" s="178"/>
-      <c r="W29" s="178"/>
-      <c r="X29" s="178"/>
-      <c r="Y29" s="178"/>
-      <c r="Z29" s="178"/>
-      <c r="AA29" s="178"/>
-      <c r="AB29" s="178"/>
-      <c r="AC29" s="178"/>
-      <c r="AD29" s="178"/>
-      <c r="AE29" s="178"/>
-      <c r="AF29" s="178"/>
-      <c r="AG29" s="178"/>
-      <c r="AH29" s="178"/>
-      <c r="AI29" s="178"/>
-      <c r="AJ29" s="178"/>
-      <c r="AK29" s="178"/>
-      <c r="AL29" s="186"/>
+      <c r="H29" s="187"/>
+      <c r="I29" s="187"/>
+      <c r="J29" s="187"/>
+      <c r="K29" s="187"/>
+      <c r="L29" s="187"/>
+      <c r="M29" s="187"/>
+      <c r="N29" s="187"/>
+      <c r="O29" s="187"/>
+      <c r="P29" s="187"/>
+      <c r="Q29" s="187"/>
+      <c r="R29" s="187"/>
+      <c r="S29" s="187"/>
+      <c r="T29" s="187"/>
+      <c r="U29" s="187"/>
+      <c r="V29" s="187"/>
+      <c r="W29" s="187"/>
+      <c r="X29" s="187"/>
+      <c r="Y29" s="187"/>
+      <c r="Z29" s="187"/>
+      <c r="AA29" s="187"/>
+      <c r="AB29" s="187"/>
+      <c r="AC29" s="187"/>
+      <c r="AD29" s="187"/>
+      <c r="AE29" s="187"/>
+      <c r="AF29" s="187"/>
+      <c r="AG29" s="187"/>
+      <c r="AH29" s="187"/>
+      <c r="AI29" s="187"/>
+      <c r="AJ29" s="187"/>
+      <c r="AK29" s="187"/>
+      <c r="AL29" s="188"/>
       <c r="AM29" s="2"/>
       <c r="AN29" s="2" t="s">
         <v>39</v>
@@ -12104,7 +12112,7 @@
         <f t="shared" si="2"/>
         <v>FFFFFFE0</v>
       </c>
-      <c r="E30" s="171"/>
+      <c r="E30" s="173"/>
       <c r="F30" s="50" t="s">
         <v>117</v>
       </c>
@@ -12114,62 +12122,62 @@
       <c r="H30" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="I30" s="169" t="s">
+      <c r="I30" s="175" t="s">
         <v>55</v>
       </c>
-      <c r="J30" s="169"/>
-      <c r="K30" s="169"/>
-      <c r="L30" s="169"/>
-      <c r="M30" s="169"/>
-      <c r="N30" s="169"/>
-      <c r="O30" s="169"/>
-      <c r="P30" s="169"/>
-      <c r="Q30" s="169"/>
-      <c r="R30" s="169"/>
-      <c r="S30" s="169"/>
-      <c r="T30" s="169"/>
-      <c r="U30" s="169"/>
-      <c r="V30" s="169"/>
+      <c r="J30" s="175"/>
+      <c r="K30" s="175"/>
+      <c r="L30" s="175"/>
+      <c r="M30" s="175"/>
+      <c r="N30" s="175"/>
+      <c r="O30" s="175"/>
+      <c r="P30" s="175"/>
+      <c r="Q30" s="175"/>
+      <c r="R30" s="175"/>
+      <c r="S30" s="175"/>
+      <c r="T30" s="175"/>
+      <c r="U30" s="175"/>
+      <c r="V30" s="175"/>
       <c r="W30" s="32">
         <v>0</v>
       </c>
       <c r="X30" s="32">
         <v>0</v>
       </c>
-      <c r="Y30" s="178" t="s">
+      <c r="Y30" s="187" t="s">
         <v>20</v>
       </c>
-      <c r="Z30" s="178"/>
+      <c r="Z30" s="187"/>
       <c r="AA30" s="32">
         <v>0</v>
       </c>
       <c r="AB30" s="32">
         <v>0</v>
       </c>
-      <c r="AC30" s="178" t="s">
+      <c r="AC30" s="187" t="s">
         <v>21</v>
       </c>
-      <c r="AD30" s="178"/>
+      <c r="AD30" s="187"/>
       <c r="AE30" s="32">
         <v>0</v>
       </c>
       <c r="AF30" s="32">
         <v>0</v>
       </c>
-      <c r="AG30" s="178" t="s">
+      <c r="AG30" s="187" t="s">
         <v>22</v>
       </c>
-      <c r="AH30" s="178"/>
+      <c r="AH30" s="187"/>
       <c r="AI30" s="32">
         <v>0</v>
       </c>
       <c r="AJ30" s="32">
         <v>0</v>
       </c>
-      <c r="AK30" s="178" t="s">
+      <c r="AK30" s="187" t="s">
         <v>23</v>
       </c>
-      <c r="AL30" s="186"/>
+      <c r="AL30" s="188"/>
       <c r="AM30" s="2"/>
       <c r="AN30" t="s">
         <v>118</v>
@@ -12188,74 +12196,74 @@
         <f t="shared" si="2"/>
         <v>FFFFFFE4</v>
       </c>
-      <c r="E31" s="171"/>
+      <c r="E31" s="173"/>
       <c r="F31" s="50" t="s">
         <v>99</v>
       </c>
       <c r="G31" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="H31" s="182" t="s">
+      <c r="H31" s="170" t="s">
         <v>60</v>
       </c>
-      <c r="I31" s="182"/>
-      <c r="J31" s="182"/>
+      <c r="I31" s="170"/>
+      <c r="J31" s="170"/>
       <c r="K31" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="L31" s="182" t="s">
+      <c r="L31" s="170" t="s">
         <v>61</v>
       </c>
-      <c r="M31" s="182"/>
-      <c r="N31" s="182"/>
+      <c r="M31" s="170"/>
+      <c r="N31" s="170"/>
       <c r="O31" s="72" t="s">
         <v>71</v>
       </c>
-      <c r="P31" s="182" t="s">
+      <c r="P31" s="170" t="s">
         <v>62</v>
       </c>
-      <c r="Q31" s="182"/>
-      <c r="R31" s="182"/>
+      <c r="Q31" s="170"/>
+      <c r="R31" s="170"/>
       <c r="S31" s="72" t="s">
         <v>70</v>
       </c>
-      <c r="T31" s="182" t="s">
+      <c r="T31" s="170" t="s">
         <v>63</v>
       </c>
-      <c r="U31" s="182"/>
-      <c r="V31" s="182"/>
+      <c r="U31" s="170"/>
+      <c r="V31" s="170"/>
       <c r="W31" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="X31" s="182" t="s">
+      <c r="X31" s="170" t="s">
         <v>56</v>
       </c>
-      <c r="Y31" s="182"/>
-      <c r="Z31" s="182"/>
+      <c r="Y31" s="170"/>
+      <c r="Z31" s="170"/>
       <c r="AA31" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="AB31" s="182" t="s">
+      <c r="AB31" s="170" t="s">
         <v>57</v>
       </c>
-      <c r="AC31" s="182"/>
-      <c r="AD31" s="182"/>
+      <c r="AC31" s="170"/>
+      <c r="AD31" s="170"/>
       <c r="AE31" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="AF31" s="182" t="s">
+      <c r="AF31" s="170" t="s">
         <v>58</v>
       </c>
-      <c r="AG31" s="182"/>
-      <c r="AH31" s="182"/>
+      <c r="AG31" s="170"/>
+      <c r="AH31" s="170"/>
       <c r="AI31" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="AJ31" s="182" t="s">
+      <c r="AJ31" s="170" t="s">
         <v>59</v>
       </c>
-      <c r="AK31" s="182"/>
-      <c r="AL31" s="193"/>
+      <c r="AK31" s="170"/>
+      <c r="AL31" s="171"/>
       <c r="AN31" s="2" t="s">
         <v>72</v>
       </c>
@@ -12273,7 +12281,7 @@
         <f t="shared" si="2"/>
         <v>FFFFFFE8</v>
       </c>
-      <c r="E32" s="171"/>
+      <c r="E32" s="173"/>
       <c r="F32" s="47" t="s">
         <v>51</v>
       </c>
@@ -12387,7 +12395,7 @@
         <f t="shared" si="2"/>
         <v>FFFFFFEC</v>
       </c>
-      <c r="E33" s="171"/>
+      <c r="E33" s="173"/>
       <c r="F33" s="47" t="s">
         <v>51</v>
       </c>
@@ -12501,7 +12509,7 @@
         <f t="shared" si="2"/>
         <v>FFFFFFF0</v>
       </c>
-      <c r="E34" s="171"/>
+      <c r="E34" s="173"/>
       <c r="F34" s="47" t="s">
         <v>51</v>
       </c>
@@ -12615,7 +12623,7 @@
         <f t="shared" si="2"/>
         <v>FFFFFFF4</v>
       </c>
-      <c r="E35" s="171"/>
+      <c r="E35" s="173"/>
       <c r="F35" s="47" t="s">
         <v>51</v>
       </c>
@@ -12729,7 +12737,7 @@
         <f t="shared" si="2"/>
         <v>FFFFFFF8</v>
       </c>
-      <c r="E36" s="171"/>
+      <c r="E36" s="173"/>
       <c r="F36" s="47" t="s">
         <v>51</v>
       </c>
@@ -12843,7 +12851,7 @@
         <f t="shared" si="2"/>
         <v>FFFFFFFC</v>
       </c>
-      <c r="E37" s="172"/>
+      <c r="E37" s="174"/>
       <c r="F37" s="52" t="s">
         <v>16</v>
       </c>
@@ -12934,11 +12942,11 @@
       <c r="AI37" s="69">
         <v>0</v>
       </c>
-      <c r="AJ37" s="187" t="s">
+      <c r="AJ37" s="189" t="s">
         <v>19</v>
       </c>
-      <c r="AK37" s="187"/>
-      <c r="AL37" s="188"/>
+      <c r="AK37" s="189"/>
+      <c r="AL37" s="190"/>
       <c r="AM37" s="31"/>
       <c r="AN37" s="2" t="s">
         <v>110</v>
@@ -12954,48 +12962,48 @@
         <v>80</v>
       </c>
       <c r="D38" s="65"/>
-      <c r="E38" s="170" t="s">
+      <c r="E38" s="172" t="s">
         <v>93</v>
       </c>
       <c r="F38" s="70" t="str">
         <f>CONCATENATE("R0.",(HEX2DEC(C38)-128)/4," or R0.",HEX2DEC(C38)/4)</f>
         <v>R0.0 or R0.32</v>
       </c>
-      <c r="G38" s="173" t="str">
+      <c r="G38" s="184" t="str">
         <f>F38</f>
         <v>R0.0 or R0.32</v>
       </c>
-      <c r="H38" s="173"/>
-      <c r="I38" s="173"/>
-      <c r="J38" s="173"/>
-      <c r="K38" s="173"/>
-      <c r="L38" s="173"/>
-      <c r="M38" s="173"/>
-      <c r="N38" s="173"/>
-      <c r="O38" s="173"/>
-      <c r="P38" s="173"/>
-      <c r="Q38" s="173"/>
-      <c r="R38" s="173"/>
-      <c r="S38" s="173"/>
-      <c r="T38" s="173"/>
-      <c r="U38" s="173"/>
-      <c r="V38" s="173"/>
-      <c r="W38" s="173"/>
-      <c r="X38" s="173"/>
-      <c r="Y38" s="173"/>
-      <c r="Z38" s="173"/>
-      <c r="AA38" s="173"/>
-      <c r="AB38" s="173"/>
-      <c r="AC38" s="173"/>
-      <c r="AD38" s="173"/>
-      <c r="AE38" s="173"/>
-      <c r="AF38" s="173"/>
-      <c r="AG38" s="173"/>
-      <c r="AH38" s="173"/>
-      <c r="AI38" s="173"/>
-      <c r="AJ38" s="173"/>
-      <c r="AK38" s="173"/>
-      <c r="AL38" s="184"/>
+      <c r="H38" s="184"/>
+      <c r="I38" s="184"/>
+      <c r="J38" s="184"/>
+      <c r="K38" s="184"/>
+      <c r="L38" s="184"/>
+      <c r="M38" s="184"/>
+      <c r="N38" s="184"/>
+      <c r="O38" s="184"/>
+      <c r="P38" s="184"/>
+      <c r="Q38" s="184"/>
+      <c r="R38" s="184"/>
+      <c r="S38" s="184"/>
+      <c r="T38" s="184"/>
+      <c r="U38" s="184"/>
+      <c r="V38" s="184"/>
+      <c r="W38" s="184"/>
+      <c r="X38" s="184"/>
+      <c r="Y38" s="184"/>
+      <c r="Z38" s="184"/>
+      <c r="AA38" s="184"/>
+      <c r="AB38" s="184"/>
+      <c r="AC38" s="184"/>
+      <c r="AD38" s="184"/>
+      <c r="AE38" s="184"/>
+      <c r="AF38" s="184"/>
+      <c r="AG38" s="184"/>
+      <c r="AH38" s="184"/>
+      <c r="AI38" s="184"/>
+      <c r="AJ38" s="184"/>
+      <c r="AK38" s="184"/>
+      <c r="AL38" s="185"/>
       <c r="AM38" s="2"/>
       <c r="AN38" s="2"/>
     </row>
@@ -13009,46 +13017,46 @@
         <v>84</v>
       </c>
       <c r="D39" s="39"/>
-      <c r="E39" s="171"/>
+      <c r="E39" s="173"/>
       <c r="F39" s="57" t="str">
         <f t="shared" ref="F39:F69" si="4">CONCATENATE("R0.",(HEX2DEC(C39)-128)/4," or R0.",HEX2DEC(C39)/4)</f>
         <v>R0.1 or R0.33</v>
       </c>
-      <c r="G39" s="180" t="str">
+      <c r="G39" s="181" t="str">
         <f t="shared" ref="G39:G68" si="5">F39</f>
         <v>R0.1 or R0.33</v>
       </c>
-      <c r="H39" s="180"/>
-      <c r="I39" s="180"/>
-      <c r="J39" s="180"/>
-      <c r="K39" s="180"/>
-      <c r="L39" s="180"/>
-      <c r="M39" s="180"/>
-      <c r="N39" s="180"/>
-      <c r="O39" s="180"/>
-      <c r="P39" s="180"/>
-      <c r="Q39" s="180"/>
-      <c r="R39" s="180"/>
-      <c r="S39" s="180"/>
-      <c r="T39" s="180"/>
-      <c r="U39" s="180"/>
-      <c r="V39" s="180"/>
-      <c r="W39" s="180"/>
-      <c r="X39" s="180"/>
-      <c r="Y39" s="180"/>
-      <c r="Z39" s="180"/>
-      <c r="AA39" s="180"/>
-      <c r="AB39" s="180"/>
-      <c r="AC39" s="180"/>
-      <c r="AD39" s="180"/>
-      <c r="AE39" s="180"/>
-      <c r="AF39" s="180"/>
-      <c r="AG39" s="180"/>
-      <c r="AH39" s="180"/>
-      <c r="AI39" s="180"/>
-      <c r="AJ39" s="180"/>
-      <c r="AK39" s="180"/>
-      <c r="AL39" s="181"/>
+      <c r="H39" s="181"/>
+      <c r="I39" s="181"/>
+      <c r="J39" s="181"/>
+      <c r="K39" s="181"/>
+      <c r="L39" s="181"/>
+      <c r="M39" s="181"/>
+      <c r="N39" s="181"/>
+      <c r="O39" s="181"/>
+      <c r="P39" s="181"/>
+      <c r="Q39" s="181"/>
+      <c r="R39" s="181"/>
+      <c r="S39" s="181"/>
+      <c r="T39" s="181"/>
+      <c r="U39" s="181"/>
+      <c r="V39" s="181"/>
+      <c r="W39" s="181"/>
+      <c r="X39" s="181"/>
+      <c r="Y39" s="181"/>
+      <c r="Z39" s="181"/>
+      <c r="AA39" s="181"/>
+      <c r="AB39" s="181"/>
+      <c r="AC39" s="181"/>
+      <c r="AD39" s="181"/>
+      <c r="AE39" s="181"/>
+      <c r="AF39" s="181"/>
+      <c r="AG39" s="181"/>
+      <c r="AH39" s="181"/>
+      <c r="AI39" s="181"/>
+      <c r="AJ39" s="181"/>
+      <c r="AK39" s="181"/>
+      <c r="AL39" s="182"/>
       <c r="AM39" s="2"/>
       <c r="AN39" s="2"/>
     </row>
@@ -13062,46 +13070,46 @@
         <v>88</v>
       </c>
       <c r="D40" s="39"/>
-      <c r="E40" s="171"/>
+      <c r="E40" s="173"/>
       <c r="F40" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.2 or R0.34</v>
       </c>
-      <c r="G40" s="180" t="str">
+      <c r="G40" s="181" t="str">
         <f t="shared" si="5"/>
         <v>R0.2 or R0.34</v>
       </c>
-      <c r="H40" s="180"/>
-      <c r="I40" s="180"/>
-      <c r="J40" s="180"/>
-      <c r="K40" s="180"/>
-      <c r="L40" s="180"/>
-      <c r="M40" s="180"/>
-      <c r="N40" s="180"/>
-      <c r="O40" s="180"/>
-      <c r="P40" s="180"/>
-      <c r="Q40" s="180"/>
-      <c r="R40" s="180"/>
-      <c r="S40" s="180"/>
-      <c r="T40" s="180"/>
-      <c r="U40" s="180"/>
-      <c r="V40" s="180"/>
-      <c r="W40" s="180"/>
-      <c r="X40" s="180"/>
-      <c r="Y40" s="180"/>
-      <c r="Z40" s="180"/>
-      <c r="AA40" s="180"/>
-      <c r="AB40" s="180"/>
-      <c r="AC40" s="180"/>
-      <c r="AD40" s="180"/>
-      <c r="AE40" s="180"/>
-      <c r="AF40" s="180"/>
-      <c r="AG40" s="180"/>
-      <c r="AH40" s="180"/>
-      <c r="AI40" s="180"/>
-      <c r="AJ40" s="180"/>
-      <c r="AK40" s="180"/>
-      <c r="AL40" s="181"/>
+      <c r="H40" s="181"/>
+      <c r="I40" s="181"/>
+      <c r="J40" s="181"/>
+      <c r="K40" s="181"/>
+      <c r="L40" s="181"/>
+      <c r="M40" s="181"/>
+      <c r="N40" s="181"/>
+      <c r="O40" s="181"/>
+      <c r="P40" s="181"/>
+      <c r="Q40" s="181"/>
+      <c r="R40" s="181"/>
+      <c r="S40" s="181"/>
+      <c r="T40" s="181"/>
+      <c r="U40" s="181"/>
+      <c r="V40" s="181"/>
+      <c r="W40" s="181"/>
+      <c r="X40" s="181"/>
+      <c r="Y40" s="181"/>
+      <c r="Z40" s="181"/>
+      <c r="AA40" s="181"/>
+      <c r="AB40" s="181"/>
+      <c r="AC40" s="181"/>
+      <c r="AD40" s="181"/>
+      <c r="AE40" s="181"/>
+      <c r="AF40" s="181"/>
+      <c r="AG40" s="181"/>
+      <c r="AH40" s="181"/>
+      <c r="AI40" s="181"/>
+      <c r="AJ40" s="181"/>
+      <c r="AK40" s="181"/>
+      <c r="AL40" s="182"/>
       <c r="AM40" s="2"/>
       <c r="AN40" s="2"/>
     </row>
@@ -13115,46 +13123,46 @@
         <v>8C</v>
       </c>
       <c r="D41" s="39"/>
-      <c r="E41" s="171"/>
+      <c r="E41" s="173"/>
       <c r="F41" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.3 or R0.35</v>
       </c>
-      <c r="G41" s="180" t="str">
+      <c r="G41" s="181" t="str">
         <f t="shared" si="5"/>
         <v>R0.3 or R0.35</v>
       </c>
-      <c r="H41" s="180"/>
-      <c r="I41" s="180"/>
-      <c r="J41" s="180"/>
-      <c r="K41" s="180"/>
-      <c r="L41" s="180"/>
-      <c r="M41" s="180"/>
-      <c r="N41" s="180"/>
-      <c r="O41" s="180"/>
-      <c r="P41" s="180"/>
-      <c r="Q41" s="180"/>
-      <c r="R41" s="180"/>
-      <c r="S41" s="180"/>
-      <c r="T41" s="180"/>
-      <c r="U41" s="180"/>
-      <c r="V41" s="180"/>
-      <c r="W41" s="180"/>
-      <c r="X41" s="180"/>
-      <c r="Y41" s="180"/>
-      <c r="Z41" s="180"/>
-      <c r="AA41" s="180"/>
-      <c r="AB41" s="180"/>
-      <c r="AC41" s="180"/>
-      <c r="AD41" s="180"/>
-      <c r="AE41" s="180"/>
-      <c r="AF41" s="180"/>
-      <c r="AG41" s="180"/>
-      <c r="AH41" s="180"/>
-      <c r="AI41" s="180"/>
-      <c r="AJ41" s="180"/>
-      <c r="AK41" s="180"/>
-      <c r="AL41" s="181"/>
+      <c r="H41" s="181"/>
+      <c r="I41" s="181"/>
+      <c r="J41" s="181"/>
+      <c r="K41" s="181"/>
+      <c r="L41" s="181"/>
+      <c r="M41" s="181"/>
+      <c r="N41" s="181"/>
+      <c r="O41" s="181"/>
+      <c r="P41" s="181"/>
+      <c r="Q41" s="181"/>
+      <c r="R41" s="181"/>
+      <c r="S41" s="181"/>
+      <c r="T41" s="181"/>
+      <c r="U41" s="181"/>
+      <c r="V41" s="181"/>
+      <c r="W41" s="181"/>
+      <c r="X41" s="181"/>
+      <c r="Y41" s="181"/>
+      <c r="Z41" s="181"/>
+      <c r="AA41" s="181"/>
+      <c r="AB41" s="181"/>
+      <c r="AC41" s="181"/>
+      <c r="AD41" s="181"/>
+      <c r="AE41" s="181"/>
+      <c r="AF41" s="181"/>
+      <c r="AG41" s="181"/>
+      <c r="AH41" s="181"/>
+      <c r="AI41" s="181"/>
+      <c r="AJ41" s="181"/>
+      <c r="AK41" s="181"/>
+      <c r="AL41" s="182"/>
       <c r="AM41" s="2"/>
       <c r="AN41" s="2"/>
     </row>
@@ -13168,46 +13176,46 @@
         <v>90</v>
       </c>
       <c r="D42" s="39"/>
-      <c r="E42" s="171"/>
+      <c r="E42" s="173"/>
       <c r="F42" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.4 or R0.36</v>
       </c>
-      <c r="G42" s="179" t="str">
+      <c r="G42" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.4 or R0.36</v>
       </c>
-      <c r="H42" s="180"/>
-      <c r="I42" s="180"/>
-      <c r="J42" s="180"/>
-      <c r="K42" s="180"/>
-      <c r="L42" s="180"/>
-      <c r="M42" s="180"/>
-      <c r="N42" s="180"/>
-      <c r="O42" s="180"/>
-      <c r="P42" s="180"/>
-      <c r="Q42" s="180"/>
-      <c r="R42" s="180"/>
-      <c r="S42" s="180"/>
-      <c r="T42" s="180"/>
-      <c r="U42" s="180"/>
-      <c r="V42" s="180"/>
-      <c r="W42" s="180"/>
-      <c r="X42" s="180"/>
-      <c r="Y42" s="180"/>
-      <c r="Z42" s="180"/>
-      <c r="AA42" s="180"/>
-      <c r="AB42" s="180"/>
-      <c r="AC42" s="180"/>
-      <c r="AD42" s="180"/>
-      <c r="AE42" s="180"/>
-      <c r="AF42" s="180"/>
-      <c r="AG42" s="180"/>
-      <c r="AH42" s="180"/>
-      <c r="AI42" s="180"/>
-      <c r="AJ42" s="180"/>
-      <c r="AK42" s="180"/>
-      <c r="AL42" s="181"/>
+      <c r="H42" s="181"/>
+      <c r="I42" s="181"/>
+      <c r="J42" s="181"/>
+      <c r="K42" s="181"/>
+      <c r="L42" s="181"/>
+      <c r="M42" s="181"/>
+      <c r="N42" s="181"/>
+      <c r="O42" s="181"/>
+      <c r="P42" s="181"/>
+      <c r="Q42" s="181"/>
+      <c r="R42" s="181"/>
+      <c r="S42" s="181"/>
+      <c r="T42" s="181"/>
+      <c r="U42" s="181"/>
+      <c r="V42" s="181"/>
+      <c r="W42" s="181"/>
+      <c r="X42" s="181"/>
+      <c r="Y42" s="181"/>
+      <c r="Z42" s="181"/>
+      <c r="AA42" s="181"/>
+      <c r="AB42" s="181"/>
+      <c r="AC42" s="181"/>
+      <c r="AD42" s="181"/>
+      <c r="AE42" s="181"/>
+      <c r="AF42" s="181"/>
+      <c r="AG42" s="181"/>
+      <c r="AH42" s="181"/>
+      <c r="AI42" s="181"/>
+      <c r="AJ42" s="181"/>
+      <c r="AK42" s="181"/>
+      <c r="AL42" s="182"/>
       <c r="AM42" s="2"/>
       <c r="AN42" s="2"/>
     </row>
@@ -13221,46 +13229,46 @@
         <v>94</v>
       </c>
       <c r="D43" s="39"/>
-      <c r="E43" s="171"/>
+      <c r="E43" s="173"/>
       <c r="F43" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.5 or R0.37</v>
       </c>
-      <c r="G43" s="179" t="str">
+      <c r="G43" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.5 or R0.37</v>
       </c>
-      <c r="H43" s="180"/>
-      <c r="I43" s="180"/>
-      <c r="J43" s="180"/>
-      <c r="K43" s="180"/>
-      <c r="L43" s="180"/>
-      <c r="M43" s="180"/>
-      <c r="N43" s="180"/>
-      <c r="O43" s="180"/>
-      <c r="P43" s="180"/>
-      <c r="Q43" s="180"/>
-      <c r="R43" s="180"/>
-      <c r="S43" s="180"/>
-      <c r="T43" s="180"/>
-      <c r="U43" s="180"/>
-      <c r="V43" s="180"/>
-      <c r="W43" s="180"/>
-      <c r="X43" s="180"/>
-      <c r="Y43" s="180"/>
-      <c r="Z43" s="180"/>
-      <c r="AA43" s="180"/>
-      <c r="AB43" s="180"/>
-      <c r="AC43" s="180"/>
-      <c r="AD43" s="180"/>
-      <c r="AE43" s="180"/>
-      <c r="AF43" s="180"/>
-      <c r="AG43" s="180"/>
-      <c r="AH43" s="180"/>
-      <c r="AI43" s="180"/>
-      <c r="AJ43" s="180"/>
-      <c r="AK43" s="180"/>
-      <c r="AL43" s="181"/>
+      <c r="H43" s="181"/>
+      <c r="I43" s="181"/>
+      <c r="J43" s="181"/>
+      <c r="K43" s="181"/>
+      <c r="L43" s="181"/>
+      <c r="M43" s="181"/>
+      <c r="N43" s="181"/>
+      <c r="O43" s="181"/>
+      <c r="P43" s="181"/>
+      <c r="Q43" s="181"/>
+      <c r="R43" s="181"/>
+      <c r="S43" s="181"/>
+      <c r="T43" s="181"/>
+      <c r="U43" s="181"/>
+      <c r="V43" s="181"/>
+      <c r="W43" s="181"/>
+      <c r="X43" s="181"/>
+      <c r="Y43" s="181"/>
+      <c r="Z43" s="181"/>
+      <c r="AA43" s="181"/>
+      <c r="AB43" s="181"/>
+      <c r="AC43" s="181"/>
+      <c r="AD43" s="181"/>
+      <c r="AE43" s="181"/>
+      <c r="AF43" s="181"/>
+      <c r="AG43" s="181"/>
+      <c r="AH43" s="181"/>
+      <c r="AI43" s="181"/>
+      <c r="AJ43" s="181"/>
+      <c r="AK43" s="181"/>
+      <c r="AL43" s="182"/>
       <c r="AM43" s="2"/>
       <c r="AN43" s="2"/>
     </row>
@@ -13274,46 +13282,46 @@
         <v>98</v>
       </c>
       <c r="D44" s="39"/>
-      <c r="E44" s="171"/>
+      <c r="E44" s="173"/>
       <c r="F44" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.6 or R0.38</v>
       </c>
-      <c r="G44" s="179" t="str">
+      <c r="G44" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.6 or R0.38</v>
       </c>
-      <c r="H44" s="180"/>
-      <c r="I44" s="180"/>
-      <c r="J44" s="180"/>
-      <c r="K44" s="180"/>
-      <c r="L44" s="180"/>
-      <c r="M44" s="180"/>
-      <c r="N44" s="180"/>
-      <c r="O44" s="180"/>
-      <c r="P44" s="180"/>
-      <c r="Q44" s="180"/>
-      <c r="R44" s="180"/>
-      <c r="S44" s="180"/>
-      <c r="T44" s="180"/>
-      <c r="U44" s="180"/>
-      <c r="V44" s="180"/>
-      <c r="W44" s="180"/>
-      <c r="X44" s="180"/>
-      <c r="Y44" s="180"/>
-      <c r="Z44" s="180"/>
-      <c r="AA44" s="180"/>
-      <c r="AB44" s="180"/>
-      <c r="AC44" s="180"/>
-      <c r="AD44" s="180"/>
-      <c r="AE44" s="180"/>
-      <c r="AF44" s="180"/>
-      <c r="AG44" s="180"/>
-      <c r="AH44" s="180"/>
-      <c r="AI44" s="180"/>
-      <c r="AJ44" s="180"/>
-      <c r="AK44" s="180"/>
-      <c r="AL44" s="181"/>
+      <c r="H44" s="181"/>
+      <c r="I44" s="181"/>
+      <c r="J44" s="181"/>
+      <c r="K44" s="181"/>
+      <c r="L44" s="181"/>
+      <c r="M44" s="181"/>
+      <c r="N44" s="181"/>
+      <c r="O44" s="181"/>
+      <c r="P44" s="181"/>
+      <c r="Q44" s="181"/>
+      <c r="R44" s="181"/>
+      <c r="S44" s="181"/>
+      <c r="T44" s="181"/>
+      <c r="U44" s="181"/>
+      <c r="V44" s="181"/>
+      <c r="W44" s="181"/>
+      <c r="X44" s="181"/>
+      <c r="Y44" s="181"/>
+      <c r="Z44" s="181"/>
+      <c r="AA44" s="181"/>
+      <c r="AB44" s="181"/>
+      <c r="AC44" s="181"/>
+      <c r="AD44" s="181"/>
+      <c r="AE44" s="181"/>
+      <c r="AF44" s="181"/>
+      <c r="AG44" s="181"/>
+      <c r="AH44" s="181"/>
+      <c r="AI44" s="181"/>
+      <c r="AJ44" s="181"/>
+      <c r="AK44" s="181"/>
+      <c r="AL44" s="182"/>
       <c r="AM44" s="2"/>
       <c r="AN44" s="2"/>
     </row>
@@ -13327,46 +13335,46 @@
         <v>9C</v>
       </c>
       <c r="D45" s="39"/>
-      <c r="E45" s="171"/>
+      <c r="E45" s="173"/>
       <c r="F45" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.7 or R0.39</v>
       </c>
-      <c r="G45" s="179" t="str">
+      <c r="G45" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.7 or R0.39</v>
       </c>
-      <c r="H45" s="180"/>
-      <c r="I45" s="180"/>
-      <c r="J45" s="180"/>
-      <c r="K45" s="180"/>
-      <c r="L45" s="180"/>
-      <c r="M45" s="180"/>
-      <c r="N45" s="180"/>
-      <c r="O45" s="180"/>
-      <c r="P45" s="180"/>
-      <c r="Q45" s="180"/>
-      <c r="R45" s="180"/>
-      <c r="S45" s="180"/>
-      <c r="T45" s="180"/>
-      <c r="U45" s="180"/>
-      <c r="V45" s="180"/>
-      <c r="W45" s="180"/>
-      <c r="X45" s="180"/>
-      <c r="Y45" s="180"/>
-      <c r="Z45" s="180"/>
-      <c r="AA45" s="180"/>
-      <c r="AB45" s="180"/>
-      <c r="AC45" s="180"/>
-      <c r="AD45" s="180"/>
-      <c r="AE45" s="180"/>
-      <c r="AF45" s="180"/>
-      <c r="AG45" s="180"/>
-      <c r="AH45" s="180"/>
-      <c r="AI45" s="180"/>
-      <c r="AJ45" s="180"/>
-      <c r="AK45" s="180"/>
-      <c r="AL45" s="181"/>
+      <c r="H45" s="181"/>
+      <c r="I45" s="181"/>
+      <c r="J45" s="181"/>
+      <c r="K45" s="181"/>
+      <c r="L45" s="181"/>
+      <c r="M45" s="181"/>
+      <c r="N45" s="181"/>
+      <c r="O45" s="181"/>
+      <c r="P45" s="181"/>
+      <c r="Q45" s="181"/>
+      <c r="R45" s="181"/>
+      <c r="S45" s="181"/>
+      <c r="T45" s="181"/>
+      <c r="U45" s="181"/>
+      <c r="V45" s="181"/>
+      <c r="W45" s="181"/>
+      <c r="X45" s="181"/>
+      <c r="Y45" s="181"/>
+      <c r="Z45" s="181"/>
+      <c r="AA45" s="181"/>
+      <c r="AB45" s="181"/>
+      <c r="AC45" s="181"/>
+      <c r="AD45" s="181"/>
+      <c r="AE45" s="181"/>
+      <c r="AF45" s="181"/>
+      <c r="AG45" s="181"/>
+      <c r="AH45" s="181"/>
+      <c r="AI45" s="181"/>
+      <c r="AJ45" s="181"/>
+      <c r="AK45" s="181"/>
+      <c r="AL45" s="182"/>
       <c r="AM45" s="2"/>
       <c r="AN45" s="2"/>
     </row>
@@ -13380,46 +13388,46 @@
         <v>A0</v>
       </c>
       <c r="D46" s="39"/>
-      <c r="E46" s="171"/>
+      <c r="E46" s="173"/>
       <c r="F46" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.8 or R0.40</v>
       </c>
-      <c r="G46" s="179" t="str">
+      <c r="G46" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.8 or R0.40</v>
       </c>
-      <c r="H46" s="180"/>
-      <c r="I46" s="180"/>
-      <c r="J46" s="180"/>
-      <c r="K46" s="180"/>
-      <c r="L46" s="180"/>
-      <c r="M46" s="180"/>
-      <c r="N46" s="180"/>
-      <c r="O46" s="180"/>
-      <c r="P46" s="180"/>
-      <c r="Q46" s="180"/>
-      <c r="R46" s="180"/>
-      <c r="S46" s="180"/>
-      <c r="T46" s="180"/>
-      <c r="U46" s="180"/>
-      <c r="V46" s="180"/>
-      <c r="W46" s="180"/>
-      <c r="X46" s="180"/>
-      <c r="Y46" s="180"/>
-      <c r="Z46" s="180"/>
-      <c r="AA46" s="180"/>
-      <c r="AB46" s="180"/>
-      <c r="AC46" s="180"/>
-      <c r="AD46" s="180"/>
-      <c r="AE46" s="180"/>
-      <c r="AF46" s="180"/>
-      <c r="AG46" s="180"/>
-      <c r="AH46" s="180"/>
-      <c r="AI46" s="180"/>
-      <c r="AJ46" s="180"/>
-      <c r="AK46" s="180"/>
-      <c r="AL46" s="181"/>
+      <c r="H46" s="181"/>
+      <c r="I46" s="181"/>
+      <c r="J46" s="181"/>
+      <c r="K46" s="181"/>
+      <c r="L46" s="181"/>
+      <c r="M46" s="181"/>
+      <c r="N46" s="181"/>
+      <c r="O46" s="181"/>
+      <c r="P46" s="181"/>
+      <c r="Q46" s="181"/>
+      <c r="R46" s="181"/>
+      <c r="S46" s="181"/>
+      <c r="T46" s="181"/>
+      <c r="U46" s="181"/>
+      <c r="V46" s="181"/>
+      <c r="W46" s="181"/>
+      <c r="X46" s="181"/>
+      <c r="Y46" s="181"/>
+      <c r="Z46" s="181"/>
+      <c r="AA46" s="181"/>
+      <c r="AB46" s="181"/>
+      <c r="AC46" s="181"/>
+      <c r="AD46" s="181"/>
+      <c r="AE46" s="181"/>
+      <c r="AF46" s="181"/>
+      <c r="AG46" s="181"/>
+      <c r="AH46" s="181"/>
+      <c r="AI46" s="181"/>
+      <c r="AJ46" s="181"/>
+      <c r="AK46" s="181"/>
+      <c r="AL46" s="182"/>
       <c r="AM46" s="2"/>
       <c r="AN46" s="2"/>
     </row>
@@ -13433,46 +13441,46 @@
         <v>A4</v>
       </c>
       <c r="D47" s="39"/>
-      <c r="E47" s="171"/>
+      <c r="E47" s="173"/>
       <c r="F47" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.9 or R0.41</v>
       </c>
-      <c r="G47" s="179" t="str">
+      <c r="G47" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.9 or R0.41</v>
       </c>
-      <c r="H47" s="180"/>
-      <c r="I47" s="180"/>
-      <c r="J47" s="180"/>
-      <c r="K47" s="180"/>
-      <c r="L47" s="180"/>
-      <c r="M47" s="180"/>
-      <c r="N47" s="180"/>
-      <c r="O47" s="180"/>
-      <c r="P47" s="180"/>
-      <c r="Q47" s="180"/>
-      <c r="R47" s="180"/>
-      <c r="S47" s="180"/>
-      <c r="T47" s="180"/>
-      <c r="U47" s="180"/>
-      <c r="V47" s="180"/>
-      <c r="W47" s="180"/>
-      <c r="X47" s="180"/>
-      <c r="Y47" s="180"/>
-      <c r="Z47" s="180"/>
-      <c r="AA47" s="180"/>
-      <c r="AB47" s="180"/>
-      <c r="AC47" s="180"/>
-      <c r="AD47" s="180"/>
-      <c r="AE47" s="180"/>
-      <c r="AF47" s="180"/>
-      <c r="AG47" s="180"/>
-      <c r="AH47" s="180"/>
-      <c r="AI47" s="180"/>
-      <c r="AJ47" s="180"/>
-      <c r="AK47" s="180"/>
-      <c r="AL47" s="181"/>
+      <c r="H47" s="181"/>
+      <c r="I47" s="181"/>
+      <c r="J47" s="181"/>
+      <c r="K47" s="181"/>
+      <c r="L47" s="181"/>
+      <c r="M47" s="181"/>
+      <c r="N47" s="181"/>
+      <c r="O47" s="181"/>
+      <c r="P47" s="181"/>
+      <c r="Q47" s="181"/>
+      <c r="R47" s="181"/>
+      <c r="S47" s="181"/>
+      <c r="T47" s="181"/>
+      <c r="U47" s="181"/>
+      <c r="V47" s="181"/>
+      <c r="W47" s="181"/>
+      <c r="X47" s="181"/>
+      <c r="Y47" s="181"/>
+      <c r="Z47" s="181"/>
+      <c r="AA47" s="181"/>
+      <c r="AB47" s="181"/>
+      <c r="AC47" s="181"/>
+      <c r="AD47" s="181"/>
+      <c r="AE47" s="181"/>
+      <c r="AF47" s="181"/>
+      <c r="AG47" s="181"/>
+      <c r="AH47" s="181"/>
+      <c r="AI47" s="181"/>
+      <c r="AJ47" s="181"/>
+      <c r="AK47" s="181"/>
+      <c r="AL47" s="182"/>
       <c r="AM47" s="2"/>
       <c r="AN47" s="2"/>
     </row>
@@ -13486,46 +13494,46 @@
         <v>A8</v>
       </c>
       <c r="D48" s="39"/>
-      <c r="E48" s="171"/>
+      <c r="E48" s="173"/>
       <c r="F48" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.10 or R0.42</v>
       </c>
-      <c r="G48" s="179" t="str">
+      <c r="G48" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.10 or R0.42</v>
       </c>
-      <c r="H48" s="180"/>
-      <c r="I48" s="180"/>
-      <c r="J48" s="180"/>
-      <c r="K48" s="180"/>
-      <c r="L48" s="180"/>
-      <c r="M48" s="180"/>
-      <c r="N48" s="180"/>
-      <c r="O48" s="180"/>
-      <c r="P48" s="180"/>
-      <c r="Q48" s="180"/>
-      <c r="R48" s="180"/>
-      <c r="S48" s="180"/>
-      <c r="T48" s="180"/>
-      <c r="U48" s="180"/>
-      <c r="V48" s="180"/>
-      <c r="W48" s="180"/>
-      <c r="X48" s="180"/>
-      <c r="Y48" s="180"/>
-      <c r="Z48" s="180"/>
-      <c r="AA48" s="180"/>
-      <c r="AB48" s="180"/>
-      <c r="AC48" s="180"/>
-      <c r="AD48" s="180"/>
-      <c r="AE48" s="180"/>
-      <c r="AF48" s="180"/>
-      <c r="AG48" s="180"/>
-      <c r="AH48" s="180"/>
-      <c r="AI48" s="180"/>
-      <c r="AJ48" s="180"/>
-      <c r="AK48" s="180"/>
-      <c r="AL48" s="181"/>
+      <c r="H48" s="181"/>
+      <c r="I48" s="181"/>
+      <c r="J48" s="181"/>
+      <c r="K48" s="181"/>
+      <c r="L48" s="181"/>
+      <c r="M48" s="181"/>
+      <c r="N48" s="181"/>
+      <c r="O48" s="181"/>
+      <c r="P48" s="181"/>
+      <c r="Q48" s="181"/>
+      <c r="R48" s="181"/>
+      <c r="S48" s="181"/>
+      <c r="T48" s="181"/>
+      <c r="U48" s="181"/>
+      <c r="V48" s="181"/>
+      <c r="W48" s="181"/>
+      <c r="X48" s="181"/>
+      <c r="Y48" s="181"/>
+      <c r="Z48" s="181"/>
+      <c r="AA48" s="181"/>
+      <c r="AB48" s="181"/>
+      <c r="AC48" s="181"/>
+      <c r="AD48" s="181"/>
+      <c r="AE48" s="181"/>
+      <c r="AF48" s="181"/>
+      <c r="AG48" s="181"/>
+      <c r="AH48" s="181"/>
+      <c r="AI48" s="181"/>
+      <c r="AJ48" s="181"/>
+      <c r="AK48" s="181"/>
+      <c r="AL48" s="182"/>
       <c r="AM48" s="2"/>
       <c r="AN48" s="2"/>
     </row>
@@ -13539,46 +13547,46 @@
         <v>AC</v>
       </c>
       <c r="D49" s="39"/>
-      <c r="E49" s="171"/>
+      <c r="E49" s="173"/>
       <c r="F49" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.11 or R0.43</v>
       </c>
-      <c r="G49" s="179" t="str">
+      <c r="G49" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.11 or R0.43</v>
       </c>
-      <c r="H49" s="180"/>
-      <c r="I49" s="180"/>
-      <c r="J49" s="180"/>
-      <c r="K49" s="180"/>
-      <c r="L49" s="180"/>
-      <c r="M49" s="180"/>
-      <c r="N49" s="180"/>
-      <c r="O49" s="180"/>
-      <c r="P49" s="180"/>
-      <c r="Q49" s="180"/>
-      <c r="R49" s="180"/>
-      <c r="S49" s="180"/>
-      <c r="T49" s="180"/>
-      <c r="U49" s="180"/>
-      <c r="V49" s="180"/>
-      <c r="W49" s="180"/>
-      <c r="X49" s="180"/>
-      <c r="Y49" s="180"/>
-      <c r="Z49" s="180"/>
-      <c r="AA49" s="180"/>
-      <c r="AB49" s="180"/>
-      <c r="AC49" s="180"/>
-      <c r="AD49" s="180"/>
-      <c r="AE49" s="180"/>
-      <c r="AF49" s="180"/>
-      <c r="AG49" s="180"/>
-      <c r="AH49" s="180"/>
-      <c r="AI49" s="180"/>
-      <c r="AJ49" s="180"/>
-      <c r="AK49" s="180"/>
-      <c r="AL49" s="181"/>
+      <c r="H49" s="181"/>
+      <c r="I49" s="181"/>
+      <c r="J49" s="181"/>
+      <c r="K49" s="181"/>
+      <c r="L49" s="181"/>
+      <c r="M49" s="181"/>
+      <c r="N49" s="181"/>
+      <c r="O49" s="181"/>
+      <c r="P49" s="181"/>
+      <c r="Q49" s="181"/>
+      <c r="R49" s="181"/>
+      <c r="S49" s="181"/>
+      <c r="T49" s="181"/>
+      <c r="U49" s="181"/>
+      <c r="V49" s="181"/>
+      <c r="W49" s="181"/>
+      <c r="X49" s="181"/>
+      <c r="Y49" s="181"/>
+      <c r="Z49" s="181"/>
+      <c r="AA49" s="181"/>
+      <c r="AB49" s="181"/>
+      <c r="AC49" s="181"/>
+      <c r="AD49" s="181"/>
+      <c r="AE49" s="181"/>
+      <c r="AF49" s="181"/>
+      <c r="AG49" s="181"/>
+      <c r="AH49" s="181"/>
+      <c r="AI49" s="181"/>
+      <c r="AJ49" s="181"/>
+      <c r="AK49" s="181"/>
+      <c r="AL49" s="182"/>
       <c r="AM49" s="2"/>
       <c r="AN49" s="2"/>
     </row>
@@ -13592,46 +13600,46 @@
         <v>B0</v>
       </c>
       <c r="D50" s="39"/>
-      <c r="E50" s="171"/>
+      <c r="E50" s="173"/>
       <c r="F50" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.12 or R0.44</v>
       </c>
-      <c r="G50" s="179" t="str">
+      <c r="G50" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.12 or R0.44</v>
       </c>
-      <c r="H50" s="180"/>
-      <c r="I50" s="180"/>
-      <c r="J50" s="180"/>
-      <c r="K50" s="180"/>
-      <c r="L50" s="180"/>
-      <c r="M50" s="180"/>
-      <c r="N50" s="180"/>
-      <c r="O50" s="180"/>
-      <c r="P50" s="180"/>
-      <c r="Q50" s="180"/>
-      <c r="R50" s="180"/>
-      <c r="S50" s="180"/>
-      <c r="T50" s="180"/>
-      <c r="U50" s="180"/>
-      <c r="V50" s="180"/>
-      <c r="W50" s="180"/>
-      <c r="X50" s="180"/>
-      <c r="Y50" s="180"/>
-      <c r="Z50" s="180"/>
-      <c r="AA50" s="180"/>
-      <c r="AB50" s="180"/>
-      <c r="AC50" s="180"/>
-      <c r="AD50" s="180"/>
-      <c r="AE50" s="180"/>
-      <c r="AF50" s="180"/>
-      <c r="AG50" s="180"/>
-      <c r="AH50" s="180"/>
-      <c r="AI50" s="180"/>
-      <c r="AJ50" s="180"/>
-      <c r="AK50" s="180"/>
-      <c r="AL50" s="181"/>
+      <c r="H50" s="181"/>
+      <c r="I50" s="181"/>
+      <c r="J50" s="181"/>
+      <c r="K50" s="181"/>
+      <c r="L50" s="181"/>
+      <c r="M50" s="181"/>
+      <c r="N50" s="181"/>
+      <c r="O50" s="181"/>
+      <c r="P50" s="181"/>
+      <c r="Q50" s="181"/>
+      <c r="R50" s="181"/>
+      <c r="S50" s="181"/>
+      <c r="T50" s="181"/>
+      <c r="U50" s="181"/>
+      <c r="V50" s="181"/>
+      <c r="W50" s="181"/>
+      <c r="X50" s="181"/>
+      <c r="Y50" s="181"/>
+      <c r="Z50" s="181"/>
+      <c r="AA50" s="181"/>
+      <c r="AB50" s="181"/>
+      <c r="AC50" s="181"/>
+      <c r="AD50" s="181"/>
+      <c r="AE50" s="181"/>
+      <c r="AF50" s="181"/>
+      <c r="AG50" s="181"/>
+      <c r="AH50" s="181"/>
+      <c r="AI50" s="181"/>
+      <c r="AJ50" s="181"/>
+      <c r="AK50" s="181"/>
+      <c r="AL50" s="182"/>
       <c r="AM50" s="2"/>
       <c r="AN50" s="2"/>
     </row>
@@ -13645,46 +13653,46 @@
         <v>B4</v>
       </c>
       <c r="D51" s="39"/>
-      <c r="E51" s="171"/>
+      <c r="E51" s="173"/>
       <c r="F51" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.13 or R0.45</v>
       </c>
-      <c r="G51" s="179" t="str">
+      <c r="G51" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.13 or R0.45</v>
       </c>
-      <c r="H51" s="180"/>
-      <c r="I51" s="180"/>
-      <c r="J51" s="180"/>
-      <c r="K51" s="180"/>
-      <c r="L51" s="180"/>
-      <c r="M51" s="180"/>
-      <c r="N51" s="180"/>
-      <c r="O51" s="180"/>
-      <c r="P51" s="180"/>
-      <c r="Q51" s="180"/>
-      <c r="R51" s="180"/>
-      <c r="S51" s="180"/>
-      <c r="T51" s="180"/>
-      <c r="U51" s="180"/>
-      <c r="V51" s="180"/>
-      <c r="W51" s="180"/>
-      <c r="X51" s="180"/>
-      <c r="Y51" s="180"/>
-      <c r="Z51" s="180"/>
-      <c r="AA51" s="180"/>
-      <c r="AB51" s="180"/>
-      <c r="AC51" s="180"/>
-      <c r="AD51" s="180"/>
-      <c r="AE51" s="180"/>
-      <c r="AF51" s="180"/>
-      <c r="AG51" s="180"/>
-      <c r="AH51" s="180"/>
-      <c r="AI51" s="180"/>
-      <c r="AJ51" s="180"/>
-      <c r="AK51" s="180"/>
-      <c r="AL51" s="181"/>
+      <c r="H51" s="181"/>
+      <c r="I51" s="181"/>
+      <c r="J51" s="181"/>
+      <c r="K51" s="181"/>
+      <c r="L51" s="181"/>
+      <c r="M51" s="181"/>
+      <c r="N51" s="181"/>
+      <c r="O51" s="181"/>
+      <c r="P51" s="181"/>
+      <c r="Q51" s="181"/>
+      <c r="R51" s="181"/>
+      <c r="S51" s="181"/>
+      <c r="T51" s="181"/>
+      <c r="U51" s="181"/>
+      <c r="V51" s="181"/>
+      <c r="W51" s="181"/>
+      <c r="X51" s="181"/>
+      <c r="Y51" s="181"/>
+      <c r="Z51" s="181"/>
+      <c r="AA51" s="181"/>
+      <c r="AB51" s="181"/>
+      <c r="AC51" s="181"/>
+      <c r="AD51" s="181"/>
+      <c r="AE51" s="181"/>
+      <c r="AF51" s="181"/>
+      <c r="AG51" s="181"/>
+      <c r="AH51" s="181"/>
+      <c r="AI51" s="181"/>
+      <c r="AJ51" s="181"/>
+      <c r="AK51" s="181"/>
+      <c r="AL51" s="182"/>
       <c r="AM51" s="2"/>
       <c r="AN51" s="2"/>
     </row>
@@ -13698,46 +13706,46 @@
         <v>B8</v>
       </c>
       <c r="D52" s="39"/>
-      <c r="E52" s="171"/>
+      <c r="E52" s="173"/>
       <c r="F52" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.14 or R0.46</v>
       </c>
-      <c r="G52" s="179" t="str">
+      <c r="G52" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.14 or R0.46</v>
       </c>
-      <c r="H52" s="180"/>
-      <c r="I52" s="180"/>
-      <c r="J52" s="180"/>
-      <c r="K52" s="180"/>
-      <c r="L52" s="180"/>
-      <c r="M52" s="180"/>
-      <c r="N52" s="180"/>
-      <c r="O52" s="180"/>
-      <c r="P52" s="180"/>
-      <c r="Q52" s="180"/>
-      <c r="R52" s="180"/>
-      <c r="S52" s="180"/>
-      <c r="T52" s="180"/>
-      <c r="U52" s="180"/>
-      <c r="V52" s="180"/>
-      <c r="W52" s="180"/>
-      <c r="X52" s="180"/>
-      <c r="Y52" s="180"/>
-      <c r="Z52" s="180"/>
-      <c r="AA52" s="180"/>
-      <c r="AB52" s="180"/>
-      <c r="AC52" s="180"/>
-      <c r="AD52" s="180"/>
-      <c r="AE52" s="180"/>
-      <c r="AF52" s="180"/>
-      <c r="AG52" s="180"/>
-      <c r="AH52" s="180"/>
-      <c r="AI52" s="180"/>
-      <c r="AJ52" s="180"/>
-      <c r="AK52" s="180"/>
-      <c r="AL52" s="181"/>
+      <c r="H52" s="181"/>
+      <c r="I52" s="181"/>
+      <c r="J52" s="181"/>
+      <c r="K52" s="181"/>
+      <c r="L52" s="181"/>
+      <c r="M52" s="181"/>
+      <c r="N52" s="181"/>
+      <c r="O52" s="181"/>
+      <c r="P52" s="181"/>
+      <c r="Q52" s="181"/>
+      <c r="R52" s="181"/>
+      <c r="S52" s="181"/>
+      <c r="T52" s="181"/>
+      <c r="U52" s="181"/>
+      <c r="V52" s="181"/>
+      <c r="W52" s="181"/>
+      <c r="X52" s="181"/>
+      <c r="Y52" s="181"/>
+      <c r="Z52" s="181"/>
+      <c r="AA52" s="181"/>
+      <c r="AB52" s="181"/>
+      <c r="AC52" s="181"/>
+      <c r="AD52" s="181"/>
+      <c r="AE52" s="181"/>
+      <c r="AF52" s="181"/>
+      <c r="AG52" s="181"/>
+      <c r="AH52" s="181"/>
+      <c r="AI52" s="181"/>
+      <c r="AJ52" s="181"/>
+      <c r="AK52" s="181"/>
+      <c r="AL52" s="182"/>
       <c r="AM52" s="2"/>
       <c r="AN52" s="2"/>
     </row>
@@ -13751,46 +13759,46 @@
         <v>BC</v>
       </c>
       <c r="D53" s="39"/>
-      <c r="E53" s="171"/>
+      <c r="E53" s="173"/>
       <c r="F53" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.15 or R0.47</v>
       </c>
-      <c r="G53" s="179" t="str">
+      <c r="G53" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.15 or R0.47</v>
       </c>
-      <c r="H53" s="180"/>
-      <c r="I53" s="180"/>
-      <c r="J53" s="180"/>
-      <c r="K53" s="180"/>
-      <c r="L53" s="180"/>
-      <c r="M53" s="180"/>
-      <c r="N53" s="180"/>
-      <c r="O53" s="180"/>
-      <c r="P53" s="180"/>
-      <c r="Q53" s="180"/>
-      <c r="R53" s="180"/>
-      <c r="S53" s="180"/>
-      <c r="T53" s="180"/>
-      <c r="U53" s="180"/>
-      <c r="V53" s="180"/>
-      <c r="W53" s="180"/>
-      <c r="X53" s="180"/>
-      <c r="Y53" s="180"/>
-      <c r="Z53" s="180"/>
-      <c r="AA53" s="180"/>
-      <c r="AB53" s="180"/>
-      <c r="AC53" s="180"/>
-      <c r="AD53" s="180"/>
-      <c r="AE53" s="180"/>
-      <c r="AF53" s="180"/>
-      <c r="AG53" s="180"/>
-      <c r="AH53" s="180"/>
-      <c r="AI53" s="180"/>
-      <c r="AJ53" s="180"/>
-      <c r="AK53" s="180"/>
-      <c r="AL53" s="181"/>
+      <c r="H53" s="181"/>
+      <c r="I53" s="181"/>
+      <c r="J53" s="181"/>
+      <c r="K53" s="181"/>
+      <c r="L53" s="181"/>
+      <c r="M53" s="181"/>
+      <c r="N53" s="181"/>
+      <c r="O53" s="181"/>
+      <c r="P53" s="181"/>
+      <c r="Q53" s="181"/>
+      <c r="R53" s="181"/>
+      <c r="S53" s="181"/>
+      <c r="T53" s="181"/>
+      <c r="U53" s="181"/>
+      <c r="V53" s="181"/>
+      <c r="W53" s="181"/>
+      <c r="X53" s="181"/>
+      <c r="Y53" s="181"/>
+      <c r="Z53" s="181"/>
+      <c r="AA53" s="181"/>
+      <c r="AB53" s="181"/>
+      <c r="AC53" s="181"/>
+      <c r="AD53" s="181"/>
+      <c r="AE53" s="181"/>
+      <c r="AF53" s="181"/>
+      <c r="AG53" s="181"/>
+      <c r="AH53" s="181"/>
+      <c r="AI53" s="181"/>
+      <c r="AJ53" s="181"/>
+      <c r="AK53" s="181"/>
+      <c r="AL53" s="182"/>
       <c r="AM53" s="2"/>
       <c r="AN53" s="2"/>
     </row>
@@ -13804,46 +13812,46 @@
         <v>C0</v>
       </c>
       <c r="D54" s="39"/>
-      <c r="E54" s="171"/>
+      <c r="E54" s="173"/>
       <c r="F54" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.16 or R0.48</v>
       </c>
-      <c r="G54" s="179" t="str">
+      <c r="G54" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.16 or R0.48</v>
       </c>
-      <c r="H54" s="180"/>
-      <c r="I54" s="180"/>
-      <c r="J54" s="180"/>
-      <c r="K54" s="180"/>
-      <c r="L54" s="180"/>
-      <c r="M54" s="180"/>
-      <c r="N54" s="180"/>
-      <c r="O54" s="180"/>
-      <c r="P54" s="180"/>
-      <c r="Q54" s="180"/>
-      <c r="R54" s="180"/>
-      <c r="S54" s="180"/>
-      <c r="T54" s="180"/>
-      <c r="U54" s="180"/>
-      <c r="V54" s="180"/>
-      <c r="W54" s="180"/>
-      <c r="X54" s="180"/>
-      <c r="Y54" s="180"/>
-      <c r="Z54" s="180"/>
-      <c r="AA54" s="180"/>
-      <c r="AB54" s="180"/>
-      <c r="AC54" s="180"/>
-      <c r="AD54" s="180"/>
-      <c r="AE54" s="180"/>
-      <c r="AF54" s="180"/>
-      <c r="AG54" s="180"/>
-      <c r="AH54" s="180"/>
-      <c r="AI54" s="180"/>
-      <c r="AJ54" s="180"/>
-      <c r="AK54" s="180"/>
-      <c r="AL54" s="181"/>
+      <c r="H54" s="181"/>
+      <c r="I54" s="181"/>
+      <c r="J54" s="181"/>
+      <c r="K54" s="181"/>
+      <c r="L54" s="181"/>
+      <c r="M54" s="181"/>
+      <c r="N54" s="181"/>
+      <c r="O54" s="181"/>
+      <c r="P54" s="181"/>
+      <c r="Q54" s="181"/>
+      <c r="R54" s="181"/>
+      <c r="S54" s="181"/>
+      <c r="T54" s="181"/>
+      <c r="U54" s="181"/>
+      <c r="V54" s="181"/>
+      <c r="W54" s="181"/>
+      <c r="X54" s="181"/>
+      <c r="Y54" s="181"/>
+      <c r="Z54" s="181"/>
+      <c r="AA54" s="181"/>
+      <c r="AB54" s="181"/>
+      <c r="AC54" s="181"/>
+      <c r="AD54" s="181"/>
+      <c r="AE54" s="181"/>
+      <c r="AF54" s="181"/>
+      <c r="AG54" s="181"/>
+      <c r="AH54" s="181"/>
+      <c r="AI54" s="181"/>
+      <c r="AJ54" s="181"/>
+      <c r="AK54" s="181"/>
+      <c r="AL54" s="182"/>
       <c r="AM54" s="2"/>
       <c r="AN54" s="2"/>
     </row>
@@ -13857,46 +13865,46 @@
         <v>C4</v>
       </c>
       <c r="D55" s="39"/>
-      <c r="E55" s="171"/>
+      <c r="E55" s="173"/>
       <c r="F55" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.17 or R0.49</v>
       </c>
-      <c r="G55" s="179" t="str">
+      <c r="G55" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.17 or R0.49</v>
       </c>
-      <c r="H55" s="180"/>
-      <c r="I55" s="180"/>
-      <c r="J55" s="180"/>
-      <c r="K55" s="180"/>
-      <c r="L55" s="180"/>
-      <c r="M55" s="180"/>
-      <c r="N55" s="180"/>
-      <c r="O55" s="180"/>
-      <c r="P55" s="180"/>
-      <c r="Q55" s="180"/>
-      <c r="R55" s="180"/>
-      <c r="S55" s="180"/>
-      <c r="T55" s="180"/>
-      <c r="U55" s="180"/>
-      <c r="V55" s="180"/>
-      <c r="W55" s="180"/>
-      <c r="X55" s="180"/>
-      <c r="Y55" s="180"/>
-      <c r="Z55" s="180"/>
-      <c r="AA55" s="180"/>
-      <c r="AB55" s="180"/>
-      <c r="AC55" s="180"/>
-      <c r="AD55" s="180"/>
-      <c r="AE55" s="180"/>
-      <c r="AF55" s="180"/>
-      <c r="AG55" s="180"/>
-      <c r="AH55" s="180"/>
-      <c r="AI55" s="180"/>
-      <c r="AJ55" s="180"/>
-      <c r="AK55" s="180"/>
-      <c r="AL55" s="181"/>
+      <c r="H55" s="181"/>
+      <c r="I55" s="181"/>
+      <c r="J55" s="181"/>
+      <c r="K55" s="181"/>
+      <c r="L55" s="181"/>
+      <c r="M55" s="181"/>
+      <c r="N55" s="181"/>
+      <c r="O55" s="181"/>
+      <c r="P55" s="181"/>
+      <c r="Q55" s="181"/>
+      <c r="R55" s="181"/>
+      <c r="S55" s="181"/>
+      <c r="T55" s="181"/>
+      <c r="U55" s="181"/>
+      <c r="V55" s="181"/>
+      <c r="W55" s="181"/>
+      <c r="X55" s="181"/>
+      <c r="Y55" s="181"/>
+      <c r="Z55" s="181"/>
+      <c r="AA55" s="181"/>
+      <c r="AB55" s="181"/>
+      <c r="AC55" s="181"/>
+      <c r="AD55" s="181"/>
+      <c r="AE55" s="181"/>
+      <c r="AF55" s="181"/>
+      <c r="AG55" s="181"/>
+      <c r="AH55" s="181"/>
+      <c r="AI55" s="181"/>
+      <c r="AJ55" s="181"/>
+      <c r="AK55" s="181"/>
+      <c r="AL55" s="182"/>
       <c r="AM55" s="2"/>
       <c r="AN55" s="2"/>
     </row>
@@ -13910,46 +13918,46 @@
         <v>C8</v>
       </c>
       <c r="D56" s="39"/>
-      <c r="E56" s="171"/>
+      <c r="E56" s="173"/>
       <c r="F56" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.18 or R0.50</v>
       </c>
-      <c r="G56" s="179" t="str">
+      <c r="G56" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.18 or R0.50</v>
       </c>
-      <c r="H56" s="180"/>
-      <c r="I56" s="180"/>
-      <c r="J56" s="180"/>
-      <c r="K56" s="180"/>
-      <c r="L56" s="180"/>
-      <c r="M56" s="180"/>
-      <c r="N56" s="180"/>
-      <c r="O56" s="180"/>
-      <c r="P56" s="180"/>
-      <c r="Q56" s="180"/>
-      <c r="R56" s="180"/>
-      <c r="S56" s="180"/>
-      <c r="T56" s="180"/>
-      <c r="U56" s="180"/>
-      <c r="V56" s="180"/>
-      <c r="W56" s="180"/>
-      <c r="X56" s="180"/>
-      <c r="Y56" s="180"/>
-      <c r="Z56" s="180"/>
-      <c r="AA56" s="180"/>
-      <c r="AB56" s="180"/>
-      <c r="AC56" s="180"/>
-      <c r="AD56" s="180"/>
-      <c r="AE56" s="180"/>
-      <c r="AF56" s="180"/>
-      <c r="AG56" s="180"/>
-      <c r="AH56" s="180"/>
-      <c r="AI56" s="180"/>
-      <c r="AJ56" s="180"/>
-      <c r="AK56" s="180"/>
-      <c r="AL56" s="181"/>
+      <c r="H56" s="181"/>
+      <c r="I56" s="181"/>
+      <c r="J56" s="181"/>
+      <c r="K56" s="181"/>
+      <c r="L56" s="181"/>
+      <c r="M56" s="181"/>
+      <c r="N56" s="181"/>
+      <c r="O56" s="181"/>
+      <c r="P56" s="181"/>
+      <c r="Q56" s="181"/>
+      <c r="R56" s="181"/>
+      <c r="S56" s="181"/>
+      <c r="T56" s="181"/>
+      <c r="U56" s="181"/>
+      <c r="V56" s="181"/>
+      <c r="W56" s="181"/>
+      <c r="X56" s="181"/>
+      <c r="Y56" s="181"/>
+      <c r="Z56" s="181"/>
+      <c r="AA56" s="181"/>
+      <c r="AB56" s="181"/>
+      <c r="AC56" s="181"/>
+      <c r="AD56" s="181"/>
+      <c r="AE56" s="181"/>
+      <c r="AF56" s="181"/>
+      <c r="AG56" s="181"/>
+      <c r="AH56" s="181"/>
+      <c r="AI56" s="181"/>
+      <c r="AJ56" s="181"/>
+      <c r="AK56" s="181"/>
+      <c r="AL56" s="182"/>
       <c r="AM56" s="2"/>
       <c r="AN56" s="2"/>
     </row>
@@ -13963,46 +13971,46 @@
         <v>CC</v>
       </c>
       <c r="D57" s="39"/>
-      <c r="E57" s="171"/>
+      <c r="E57" s="173"/>
       <c r="F57" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.19 or R0.51</v>
       </c>
-      <c r="G57" s="179" t="str">
+      <c r="G57" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.19 or R0.51</v>
       </c>
-      <c r="H57" s="180"/>
-      <c r="I57" s="180"/>
-      <c r="J57" s="180"/>
-      <c r="K57" s="180"/>
-      <c r="L57" s="180"/>
-      <c r="M57" s="180"/>
-      <c r="N57" s="180"/>
-      <c r="O57" s="180"/>
-      <c r="P57" s="180"/>
-      <c r="Q57" s="180"/>
-      <c r="R57" s="180"/>
-      <c r="S57" s="180"/>
-      <c r="T57" s="180"/>
-      <c r="U57" s="180"/>
-      <c r="V57" s="180"/>
-      <c r="W57" s="180"/>
-      <c r="X57" s="180"/>
-      <c r="Y57" s="180"/>
-      <c r="Z57" s="180"/>
-      <c r="AA57" s="180"/>
-      <c r="AB57" s="180"/>
-      <c r="AC57" s="180"/>
-      <c r="AD57" s="180"/>
-      <c r="AE57" s="180"/>
-      <c r="AF57" s="180"/>
-      <c r="AG57" s="180"/>
-      <c r="AH57" s="180"/>
-      <c r="AI57" s="180"/>
-      <c r="AJ57" s="180"/>
-      <c r="AK57" s="180"/>
-      <c r="AL57" s="181"/>
+      <c r="H57" s="181"/>
+      <c r="I57" s="181"/>
+      <c r="J57" s="181"/>
+      <c r="K57" s="181"/>
+      <c r="L57" s="181"/>
+      <c r="M57" s="181"/>
+      <c r="N57" s="181"/>
+      <c r="O57" s="181"/>
+      <c r="P57" s="181"/>
+      <c r="Q57" s="181"/>
+      <c r="R57" s="181"/>
+      <c r="S57" s="181"/>
+      <c r="T57" s="181"/>
+      <c r="U57" s="181"/>
+      <c r="V57" s="181"/>
+      <c r="W57" s="181"/>
+      <c r="X57" s="181"/>
+      <c r="Y57" s="181"/>
+      <c r="Z57" s="181"/>
+      <c r="AA57" s="181"/>
+      <c r="AB57" s="181"/>
+      <c r="AC57" s="181"/>
+      <c r="AD57" s="181"/>
+      <c r="AE57" s="181"/>
+      <c r="AF57" s="181"/>
+      <c r="AG57" s="181"/>
+      <c r="AH57" s="181"/>
+      <c r="AI57" s="181"/>
+      <c r="AJ57" s="181"/>
+      <c r="AK57" s="181"/>
+      <c r="AL57" s="182"/>
       <c r="AM57" s="2"/>
       <c r="AN57" s="2"/>
     </row>
@@ -14016,46 +14024,46 @@
         <v>D0</v>
       </c>
       <c r="D58" s="39"/>
-      <c r="E58" s="171"/>
+      <c r="E58" s="173"/>
       <c r="F58" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.20 or R0.52</v>
       </c>
-      <c r="G58" s="179" t="str">
+      <c r="G58" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.20 or R0.52</v>
       </c>
-      <c r="H58" s="180"/>
-      <c r="I58" s="180"/>
-      <c r="J58" s="180"/>
-      <c r="K58" s="180"/>
-      <c r="L58" s="180"/>
-      <c r="M58" s="180"/>
-      <c r="N58" s="180"/>
-      <c r="O58" s="180"/>
-      <c r="P58" s="180"/>
-      <c r="Q58" s="180"/>
-      <c r="R58" s="180"/>
-      <c r="S58" s="180"/>
-      <c r="T58" s="180"/>
-      <c r="U58" s="180"/>
-      <c r="V58" s="180"/>
-      <c r="W58" s="180"/>
-      <c r="X58" s="180"/>
-      <c r="Y58" s="180"/>
-      <c r="Z58" s="180"/>
-      <c r="AA58" s="180"/>
-      <c r="AB58" s="180"/>
-      <c r="AC58" s="180"/>
-      <c r="AD58" s="180"/>
-      <c r="AE58" s="180"/>
-      <c r="AF58" s="180"/>
-      <c r="AG58" s="180"/>
-      <c r="AH58" s="180"/>
-      <c r="AI58" s="180"/>
-      <c r="AJ58" s="180"/>
-      <c r="AK58" s="180"/>
-      <c r="AL58" s="181"/>
+      <c r="H58" s="181"/>
+      <c r="I58" s="181"/>
+      <c r="J58" s="181"/>
+      <c r="K58" s="181"/>
+      <c r="L58" s="181"/>
+      <c r="M58" s="181"/>
+      <c r="N58" s="181"/>
+      <c r="O58" s="181"/>
+      <c r="P58" s="181"/>
+      <c r="Q58" s="181"/>
+      <c r="R58" s="181"/>
+      <c r="S58" s="181"/>
+      <c r="T58" s="181"/>
+      <c r="U58" s="181"/>
+      <c r="V58" s="181"/>
+      <c r="W58" s="181"/>
+      <c r="X58" s="181"/>
+      <c r="Y58" s="181"/>
+      <c r="Z58" s="181"/>
+      <c r="AA58" s="181"/>
+      <c r="AB58" s="181"/>
+      <c r="AC58" s="181"/>
+      <c r="AD58" s="181"/>
+      <c r="AE58" s="181"/>
+      <c r="AF58" s="181"/>
+      <c r="AG58" s="181"/>
+      <c r="AH58" s="181"/>
+      <c r="AI58" s="181"/>
+      <c r="AJ58" s="181"/>
+      <c r="AK58" s="181"/>
+      <c r="AL58" s="182"/>
       <c r="AM58" s="2"/>
       <c r="AN58" s="2"/>
     </row>
@@ -14069,46 +14077,46 @@
         <v>D4</v>
       </c>
       <c r="D59" s="39"/>
-      <c r="E59" s="171"/>
+      <c r="E59" s="173"/>
       <c r="F59" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.21 or R0.53</v>
       </c>
-      <c r="G59" s="179" t="str">
+      <c r="G59" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.21 or R0.53</v>
       </c>
-      <c r="H59" s="180"/>
-      <c r="I59" s="180"/>
-      <c r="J59" s="180"/>
-      <c r="K59" s="180"/>
-      <c r="L59" s="180"/>
-      <c r="M59" s="180"/>
-      <c r="N59" s="180"/>
-      <c r="O59" s="180"/>
-      <c r="P59" s="180"/>
-      <c r="Q59" s="180"/>
-      <c r="R59" s="180"/>
-      <c r="S59" s="180"/>
-      <c r="T59" s="180"/>
-      <c r="U59" s="180"/>
-      <c r="V59" s="180"/>
-      <c r="W59" s="180"/>
-      <c r="X59" s="180"/>
-      <c r="Y59" s="180"/>
-      <c r="Z59" s="180"/>
-      <c r="AA59" s="180"/>
-      <c r="AB59" s="180"/>
-      <c r="AC59" s="180"/>
-      <c r="AD59" s="180"/>
-      <c r="AE59" s="180"/>
-      <c r="AF59" s="180"/>
-      <c r="AG59" s="180"/>
-      <c r="AH59" s="180"/>
-      <c r="AI59" s="180"/>
-      <c r="AJ59" s="180"/>
-      <c r="AK59" s="180"/>
-      <c r="AL59" s="181"/>
+      <c r="H59" s="181"/>
+      <c r="I59" s="181"/>
+      <c r="J59" s="181"/>
+      <c r="K59" s="181"/>
+      <c r="L59" s="181"/>
+      <c r="M59" s="181"/>
+      <c r="N59" s="181"/>
+      <c r="O59" s="181"/>
+      <c r="P59" s="181"/>
+      <c r="Q59" s="181"/>
+      <c r="R59" s="181"/>
+      <c r="S59" s="181"/>
+      <c r="T59" s="181"/>
+      <c r="U59" s="181"/>
+      <c r="V59" s="181"/>
+      <c r="W59" s="181"/>
+      <c r="X59" s="181"/>
+      <c r="Y59" s="181"/>
+      <c r="Z59" s="181"/>
+      <c r="AA59" s="181"/>
+      <c r="AB59" s="181"/>
+      <c r="AC59" s="181"/>
+      <c r="AD59" s="181"/>
+      <c r="AE59" s="181"/>
+      <c r="AF59" s="181"/>
+      <c r="AG59" s="181"/>
+      <c r="AH59" s="181"/>
+      <c r="AI59" s="181"/>
+      <c r="AJ59" s="181"/>
+      <c r="AK59" s="181"/>
+      <c r="AL59" s="182"/>
       <c r="AM59" s="2"/>
       <c r="AN59" s="2"/>
     </row>
@@ -14122,46 +14130,46 @@
         <v>D8</v>
       </c>
       <c r="D60" s="39"/>
-      <c r="E60" s="171"/>
+      <c r="E60" s="173"/>
       <c r="F60" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.22 or R0.54</v>
       </c>
-      <c r="G60" s="179" t="str">
+      <c r="G60" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.22 or R0.54</v>
       </c>
-      <c r="H60" s="180"/>
-      <c r="I60" s="180"/>
-      <c r="J60" s="180"/>
-      <c r="K60" s="180"/>
-      <c r="L60" s="180"/>
-      <c r="M60" s="180"/>
-      <c r="N60" s="180"/>
-      <c r="O60" s="180"/>
-      <c r="P60" s="180"/>
-      <c r="Q60" s="180"/>
-      <c r="R60" s="180"/>
-      <c r="S60" s="180"/>
-      <c r="T60" s="180"/>
-      <c r="U60" s="180"/>
-      <c r="V60" s="180"/>
-      <c r="W60" s="180"/>
-      <c r="X60" s="180"/>
-      <c r="Y60" s="180"/>
-      <c r="Z60" s="180"/>
-      <c r="AA60" s="180"/>
-      <c r="AB60" s="180"/>
-      <c r="AC60" s="180"/>
-      <c r="AD60" s="180"/>
-      <c r="AE60" s="180"/>
-      <c r="AF60" s="180"/>
-      <c r="AG60" s="180"/>
-      <c r="AH60" s="180"/>
-      <c r="AI60" s="180"/>
-      <c r="AJ60" s="180"/>
-      <c r="AK60" s="180"/>
-      <c r="AL60" s="181"/>
+      <c r="H60" s="181"/>
+      <c r="I60" s="181"/>
+      <c r="J60" s="181"/>
+      <c r="K60" s="181"/>
+      <c r="L60" s="181"/>
+      <c r="M60" s="181"/>
+      <c r="N60" s="181"/>
+      <c r="O60" s="181"/>
+      <c r="P60" s="181"/>
+      <c r="Q60" s="181"/>
+      <c r="R60" s="181"/>
+      <c r="S60" s="181"/>
+      <c r="T60" s="181"/>
+      <c r="U60" s="181"/>
+      <c r="V60" s="181"/>
+      <c r="W60" s="181"/>
+      <c r="X60" s="181"/>
+      <c r="Y60" s="181"/>
+      <c r="Z60" s="181"/>
+      <c r="AA60" s="181"/>
+      <c r="AB60" s="181"/>
+      <c r="AC60" s="181"/>
+      <c r="AD60" s="181"/>
+      <c r="AE60" s="181"/>
+      <c r="AF60" s="181"/>
+      <c r="AG60" s="181"/>
+      <c r="AH60" s="181"/>
+      <c r="AI60" s="181"/>
+      <c r="AJ60" s="181"/>
+      <c r="AK60" s="181"/>
+      <c r="AL60" s="182"/>
       <c r="AM60" s="2"/>
       <c r="AN60" s="2"/>
     </row>
@@ -14175,46 +14183,46 @@
         <v>DC</v>
       </c>
       <c r="D61" s="39"/>
-      <c r="E61" s="171"/>
+      <c r="E61" s="173"/>
       <c r="F61" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.23 or R0.55</v>
       </c>
-      <c r="G61" s="179" t="str">
+      <c r="G61" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.23 or R0.55</v>
       </c>
-      <c r="H61" s="180"/>
-      <c r="I61" s="180"/>
-      <c r="J61" s="180"/>
-      <c r="K61" s="180"/>
-      <c r="L61" s="180"/>
-      <c r="M61" s="180"/>
-      <c r="N61" s="180"/>
-      <c r="O61" s="180"/>
-      <c r="P61" s="180"/>
-      <c r="Q61" s="180"/>
-      <c r="R61" s="180"/>
-      <c r="S61" s="180"/>
-      <c r="T61" s="180"/>
-      <c r="U61" s="180"/>
-      <c r="V61" s="180"/>
-      <c r="W61" s="180"/>
-      <c r="X61" s="180"/>
-      <c r="Y61" s="180"/>
-      <c r="Z61" s="180"/>
-      <c r="AA61" s="180"/>
-      <c r="AB61" s="180"/>
-      <c r="AC61" s="180"/>
-      <c r="AD61" s="180"/>
-      <c r="AE61" s="180"/>
-      <c r="AF61" s="180"/>
-      <c r="AG61" s="180"/>
-      <c r="AH61" s="180"/>
-      <c r="AI61" s="180"/>
-      <c r="AJ61" s="180"/>
-      <c r="AK61" s="180"/>
-      <c r="AL61" s="181"/>
+      <c r="H61" s="181"/>
+      <c r="I61" s="181"/>
+      <c r="J61" s="181"/>
+      <c r="K61" s="181"/>
+      <c r="L61" s="181"/>
+      <c r="M61" s="181"/>
+      <c r="N61" s="181"/>
+      <c r="O61" s="181"/>
+      <c r="P61" s="181"/>
+      <c r="Q61" s="181"/>
+      <c r="R61" s="181"/>
+      <c r="S61" s="181"/>
+      <c r="T61" s="181"/>
+      <c r="U61" s="181"/>
+      <c r="V61" s="181"/>
+      <c r="W61" s="181"/>
+      <c r="X61" s="181"/>
+      <c r="Y61" s="181"/>
+      <c r="Z61" s="181"/>
+      <c r="AA61" s="181"/>
+      <c r="AB61" s="181"/>
+      <c r="AC61" s="181"/>
+      <c r="AD61" s="181"/>
+      <c r="AE61" s="181"/>
+      <c r="AF61" s="181"/>
+      <c r="AG61" s="181"/>
+      <c r="AH61" s="181"/>
+      <c r="AI61" s="181"/>
+      <c r="AJ61" s="181"/>
+      <c r="AK61" s="181"/>
+      <c r="AL61" s="182"/>
       <c r="AM61" s="2"/>
       <c r="AN61" s="2"/>
     </row>
@@ -14228,46 +14236,46 @@
         <v>E0</v>
       </c>
       <c r="D62" s="39"/>
-      <c r="E62" s="171"/>
+      <c r="E62" s="173"/>
       <c r="F62" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.24 or R0.56</v>
       </c>
-      <c r="G62" s="179" t="str">
+      <c r="G62" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.24 or R0.56</v>
       </c>
-      <c r="H62" s="180"/>
-      <c r="I62" s="180"/>
-      <c r="J62" s="180"/>
-      <c r="K62" s="180"/>
-      <c r="L62" s="180"/>
-      <c r="M62" s="180"/>
-      <c r="N62" s="180"/>
-      <c r="O62" s="180"/>
-      <c r="P62" s="180"/>
-      <c r="Q62" s="180"/>
-      <c r="R62" s="180"/>
-      <c r="S62" s="180"/>
-      <c r="T62" s="180"/>
-      <c r="U62" s="180"/>
-      <c r="V62" s="180"/>
-      <c r="W62" s="180"/>
-      <c r="X62" s="180"/>
-      <c r="Y62" s="180"/>
-      <c r="Z62" s="180"/>
-      <c r="AA62" s="180"/>
-      <c r="AB62" s="180"/>
-      <c r="AC62" s="180"/>
-      <c r="AD62" s="180"/>
-      <c r="AE62" s="180"/>
-      <c r="AF62" s="180"/>
-      <c r="AG62" s="180"/>
-      <c r="AH62" s="180"/>
-      <c r="AI62" s="180"/>
-      <c r="AJ62" s="180"/>
-      <c r="AK62" s="180"/>
-      <c r="AL62" s="181"/>
+      <c r="H62" s="181"/>
+      <c r="I62" s="181"/>
+      <c r="J62" s="181"/>
+      <c r="K62" s="181"/>
+      <c r="L62" s="181"/>
+      <c r="M62" s="181"/>
+      <c r="N62" s="181"/>
+      <c r="O62" s="181"/>
+      <c r="P62" s="181"/>
+      <c r="Q62" s="181"/>
+      <c r="R62" s="181"/>
+      <c r="S62" s="181"/>
+      <c r="T62" s="181"/>
+      <c r="U62" s="181"/>
+      <c r="V62" s="181"/>
+      <c r="W62" s="181"/>
+      <c r="X62" s="181"/>
+      <c r="Y62" s="181"/>
+      <c r="Z62" s="181"/>
+      <c r="AA62" s="181"/>
+      <c r="AB62" s="181"/>
+      <c r="AC62" s="181"/>
+      <c r="AD62" s="181"/>
+      <c r="AE62" s="181"/>
+      <c r="AF62" s="181"/>
+      <c r="AG62" s="181"/>
+      <c r="AH62" s="181"/>
+      <c r="AI62" s="181"/>
+      <c r="AJ62" s="181"/>
+      <c r="AK62" s="181"/>
+      <c r="AL62" s="182"/>
       <c r="AM62" s="2"/>
       <c r="AN62" s="2"/>
     </row>
@@ -14281,46 +14289,46 @@
         <v>E4</v>
       </c>
       <c r="D63" s="39"/>
-      <c r="E63" s="171"/>
+      <c r="E63" s="173"/>
       <c r="F63" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.25 or R0.57</v>
       </c>
-      <c r="G63" s="179" t="str">
+      <c r="G63" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.25 or R0.57</v>
       </c>
-      <c r="H63" s="180"/>
-      <c r="I63" s="180"/>
-      <c r="J63" s="180"/>
-      <c r="K63" s="180"/>
-      <c r="L63" s="180"/>
-      <c r="M63" s="180"/>
-      <c r="N63" s="180"/>
-      <c r="O63" s="180"/>
-      <c r="P63" s="180"/>
-      <c r="Q63" s="180"/>
-      <c r="R63" s="180"/>
-      <c r="S63" s="180"/>
-      <c r="T63" s="180"/>
-      <c r="U63" s="180"/>
-      <c r="V63" s="180"/>
-      <c r="W63" s="180"/>
-      <c r="X63" s="180"/>
-      <c r="Y63" s="180"/>
-      <c r="Z63" s="180"/>
-      <c r="AA63" s="180"/>
-      <c r="AB63" s="180"/>
-      <c r="AC63" s="180"/>
-      <c r="AD63" s="180"/>
-      <c r="AE63" s="180"/>
-      <c r="AF63" s="180"/>
-      <c r="AG63" s="180"/>
-      <c r="AH63" s="180"/>
-      <c r="AI63" s="180"/>
-      <c r="AJ63" s="180"/>
-      <c r="AK63" s="180"/>
-      <c r="AL63" s="181"/>
+      <c r="H63" s="181"/>
+      <c r="I63" s="181"/>
+      <c r="J63" s="181"/>
+      <c r="K63" s="181"/>
+      <c r="L63" s="181"/>
+      <c r="M63" s="181"/>
+      <c r="N63" s="181"/>
+      <c r="O63" s="181"/>
+      <c r="P63" s="181"/>
+      <c r="Q63" s="181"/>
+      <c r="R63" s="181"/>
+      <c r="S63" s="181"/>
+      <c r="T63" s="181"/>
+      <c r="U63" s="181"/>
+      <c r="V63" s="181"/>
+      <c r="W63" s="181"/>
+      <c r="X63" s="181"/>
+      <c r="Y63" s="181"/>
+      <c r="Z63" s="181"/>
+      <c r="AA63" s="181"/>
+      <c r="AB63" s="181"/>
+      <c r="AC63" s="181"/>
+      <c r="AD63" s="181"/>
+      <c r="AE63" s="181"/>
+      <c r="AF63" s="181"/>
+      <c r="AG63" s="181"/>
+      <c r="AH63" s="181"/>
+      <c r="AI63" s="181"/>
+      <c r="AJ63" s="181"/>
+      <c r="AK63" s="181"/>
+      <c r="AL63" s="182"/>
       <c r="AM63" s="2"/>
       <c r="AN63" s="2"/>
     </row>
@@ -14334,46 +14342,46 @@
         <v>E8</v>
       </c>
       <c r="D64" s="39"/>
-      <c r="E64" s="171"/>
+      <c r="E64" s="173"/>
       <c r="F64" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.26 or R0.58</v>
       </c>
-      <c r="G64" s="179" t="str">
+      <c r="G64" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.26 or R0.58</v>
       </c>
-      <c r="H64" s="180"/>
-      <c r="I64" s="180"/>
-      <c r="J64" s="180"/>
-      <c r="K64" s="180"/>
-      <c r="L64" s="180"/>
-      <c r="M64" s="180"/>
-      <c r="N64" s="180"/>
-      <c r="O64" s="180"/>
-      <c r="P64" s="180"/>
-      <c r="Q64" s="180"/>
-      <c r="R64" s="180"/>
-      <c r="S64" s="180"/>
-      <c r="T64" s="180"/>
-      <c r="U64" s="180"/>
-      <c r="V64" s="180"/>
-      <c r="W64" s="180"/>
-      <c r="X64" s="180"/>
-      <c r="Y64" s="180"/>
-      <c r="Z64" s="180"/>
-      <c r="AA64" s="180"/>
-      <c r="AB64" s="180"/>
-      <c r="AC64" s="180"/>
-      <c r="AD64" s="180"/>
-      <c r="AE64" s="180"/>
-      <c r="AF64" s="180"/>
-      <c r="AG64" s="180"/>
-      <c r="AH64" s="180"/>
-      <c r="AI64" s="180"/>
-      <c r="AJ64" s="180"/>
-      <c r="AK64" s="180"/>
-      <c r="AL64" s="181"/>
+      <c r="H64" s="181"/>
+      <c r="I64" s="181"/>
+      <c r="J64" s="181"/>
+      <c r="K64" s="181"/>
+      <c r="L64" s="181"/>
+      <c r="M64" s="181"/>
+      <c r="N64" s="181"/>
+      <c r="O64" s="181"/>
+      <c r="P64" s="181"/>
+      <c r="Q64" s="181"/>
+      <c r="R64" s="181"/>
+      <c r="S64" s="181"/>
+      <c r="T64" s="181"/>
+      <c r="U64" s="181"/>
+      <c r="V64" s="181"/>
+      <c r="W64" s="181"/>
+      <c r="X64" s="181"/>
+      <c r="Y64" s="181"/>
+      <c r="Z64" s="181"/>
+      <c r="AA64" s="181"/>
+      <c r="AB64" s="181"/>
+      <c r="AC64" s="181"/>
+      <c r="AD64" s="181"/>
+      <c r="AE64" s="181"/>
+      <c r="AF64" s="181"/>
+      <c r="AG64" s="181"/>
+      <c r="AH64" s="181"/>
+      <c r="AI64" s="181"/>
+      <c r="AJ64" s="181"/>
+      <c r="AK64" s="181"/>
+      <c r="AL64" s="182"/>
       <c r="AM64" s="2"/>
       <c r="AN64" s="2"/>
     </row>
@@ -14387,46 +14395,46 @@
         <v>EC</v>
       </c>
       <c r="D65" s="39"/>
-      <c r="E65" s="171"/>
+      <c r="E65" s="173"/>
       <c r="F65" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.27 or R0.59</v>
       </c>
-      <c r="G65" s="179" t="str">
+      <c r="G65" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.27 or R0.59</v>
       </c>
-      <c r="H65" s="180"/>
-      <c r="I65" s="180"/>
-      <c r="J65" s="180"/>
-      <c r="K65" s="180"/>
-      <c r="L65" s="180"/>
-      <c r="M65" s="180"/>
-      <c r="N65" s="180"/>
-      <c r="O65" s="180"/>
-      <c r="P65" s="180"/>
-      <c r="Q65" s="180"/>
-      <c r="R65" s="180"/>
-      <c r="S65" s="180"/>
-      <c r="T65" s="180"/>
-      <c r="U65" s="180"/>
-      <c r="V65" s="180"/>
-      <c r="W65" s="180"/>
-      <c r="X65" s="180"/>
-      <c r="Y65" s="180"/>
-      <c r="Z65" s="180"/>
-      <c r="AA65" s="180"/>
-      <c r="AB65" s="180"/>
-      <c r="AC65" s="180"/>
-      <c r="AD65" s="180"/>
-      <c r="AE65" s="180"/>
-      <c r="AF65" s="180"/>
-      <c r="AG65" s="180"/>
-      <c r="AH65" s="180"/>
-      <c r="AI65" s="180"/>
-      <c r="AJ65" s="180"/>
-      <c r="AK65" s="180"/>
-      <c r="AL65" s="181"/>
+      <c r="H65" s="181"/>
+      <c r="I65" s="181"/>
+      <c r="J65" s="181"/>
+      <c r="K65" s="181"/>
+      <c r="L65" s="181"/>
+      <c r="M65" s="181"/>
+      <c r="N65" s="181"/>
+      <c r="O65" s="181"/>
+      <c r="P65" s="181"/>
+      <c r="Q65" s="181"/>
+      <c r="R65" s="181"/>
+      <c r="S65" s="181"/>
+      <c r="T65" s="181"/>
+      <c r="U65" s="181"/>
+      <c r="V65" s="181"/>
+      <c r="W65" s="181"/>
+      <c r="X65" s="181"/>
+      <c r="Y65" s="181"/>
+      <c r="Z65" s="181"/>
+      <c r="AA65" s="181"/>
+      <c r="AB65" s="181"/>
+      <c r="AC65" s="181"/>
+      <c r="AD65" s="181"/>
+      <c r="AE65" s="181"/>
+      <c r="AF65" s="181"/>
+      <c r="AG65" s="181"/>
+      <c r="AH65" s="181"/>
+      <c r="AI65" s="181"/>
+      <c r="AJ65" s="181"/>
+      <c r="AK65" s="181"/>
+      <c r="AL65" s="182"/>
       <c r="AM65" s="2"/>
       <c r="AN65" s="2"/>
     </row>
@@ -14440,46 +14448,46 @@
         <v>F0</v>
       </c>
       <c r="D66" s="39"/>
-      <c r="E66" s="171"/>
+      <c r="E66" s="173"/>
       <c r="F66" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.28 or R0.60</v>
       </c>
-      <c r="G66" s="179" t="str">
+      <c r="G66" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.28 or R0.60</v>
       </c>
-      <c r="H66" s="180"/>
-      <c r="I66" s="180"/>
-      <c r="J66" s="180"/>
-      <c r="K66" s="180"/>
-      <c r="L66" s="180"/>
-      <c r="M66" s="180"/>
-      <c r="N66" s="180"/>
-      <c r="O66" s="180"/>
-      <c r="P66" s="180"/>
-      <c r="Q66" s="180"/>
-      <c r="R66" s="180"/>
-      <c r="S66" s="180"/>
-      <c r="T66" s="180"/>
-      <c r="U66" s="180"/>
-      <c r="V66" s="180"/>
-      <c r="W66" s="180"/>
-      <c r="X66" s="180"/>
-      <c r="Y66" s="180"/>
-      <c r="Z66" s="180"/>
-      <c r="AA66" s="180"/>
-      <c r="AB66" s="180"/>
-      <c r="AC66" s="180"/>
-      <c r="AD66" s="180"/>
-      <c r="AE66" s="180"/>
-      <c r="AF66" s="180"/>
-      <c r="AG66" s="180"/>
-      <c r="AH66" s="180"/>
-      <c r="AI66" s="180"/>
-      <c r="AJ66" s="180"/>
-      <c r="AK66" s="180"/>
-      <c r="AL66" s="181"/>
+      <c r="H66" s="181"/>
+      <c r="I66" s="181"/>
+      <c r="J66" s="181"/>
+      <c r="K66" s="181"/>
+      <c r="L66" s="181"/>
+      <c r="M66" s="181"/>
+      <c r="N66" s="181"/>
+      <c r="O66" s="181"/>
+      <c r="P66" s="181"/>
+      <c r="Q66" s="181"/>
+      <c r="R66" s="181"/>
+      <c r="S66" s="181"/>
+      <c r="T66" s="181"/>
+      <c r="U66" s="181"/>
+      <c r="V66" s="181"/>
+      <c r="W66" s="181"/>
+      <c r="X66" s="181"/>
+      <c r="Y66" s="181"/>
+      <c r="Z66" s="181"/>
+      <c r="AA66" s="181"/>
+      <c r="AB66" s="181"/>
+      <c r="AC66" s="181"/>
+      <c r="AD66" s="181"/>
+      <c r="AE66" s="181"/>
+      <c r="AF66" s="181"/>
+      <c r="AG66" s="181"/>
+      <c r="AH66" s="181"/>
+      <c r="AI66" s="181"/>
+      <c r="AJ66" s="181"/>
+      <c r="AK66" s="181"/>
+      <c r="AL66" s="182"/>
       <c r="AM66" s="2"/>
       <c r="AN66" s="2"/>
     </row>
@@ -14493,46 +14501,46 @@
         <v>F4</v>
       </c>
       <c r="D67" s="39"/>
-      <c r="E67" s="171"/>
+      <c r="E67" s="173"/>
       <c r="F67" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.29 or R0.61</v>
       </c>
-      <c r="G67" s="179" t="str">
+      <c r="G67" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.29 or R0.61</v>
       </c>
-      <c r="H67" s="180"/>
-      <c r="I67" s="180"/>
-      <c r="J67" s="180"/>
-      <c r="K67" s="180"/>
-      <c r="L67" s="180"/>
-      <c r="M67" s="180"/>
-      <c r="N67" s="180"/>
-      <c r="O67" s="180"/>
-      <c r="P67" s="180"/>
-      <c r="Q67" s="180"/>
-      <c r="R67" s="180"/>
-      <c r="S67" s="180"/>
-      <c r="T67" s="180"/>
-      <c r="U67" s="180"/>
-      <c r="V67" s="180"/>
-      <c r="W67" s="180"/>
-      <c r="X67" s="180"/>
-      <c r="Y67" s="180"/>
-      <c r="Z67" s="180"/>
-      <c r="AA67" s="180"/>
-      <c r="AB67" s="180"/>
-      <c r="AC67" s="180"/>
-      <c r="AD67" s="180"/>
-      <c r="AE67" s="180"/>
-      <c r="AF67" s="180"/>
-      <c r="AG67" s="180"/>
-      <c r="AH67" s="180"/>
-      <c r="AI67" s="180"/>
-      <c r="AJ67" s="180"/>
-      <c r="AK67" s="180"/>
-      <c r="AL67" s="181"/>
+      <c r="H67" s="181"/>
+      <c r="I67" s="181"/>
+      <c r="J67" s="181"/>
+      <c r="K67" s="181"/>
+      <c r="L67" s="181"/>
+      <c r="M67" s="181"/>
+      <c r="N67" s="181"/>
+      <c r="O67" s="181"/>
+      <c r="P67" s="181"/>
+      <c r="Q67" s="181"/>
+      <c r="R67" s="181"/>
+      <c r="S67" s="181"/>
+      <c r="T67" s="181"/>
+      <c r="U67" s="181"/>
+      <c r="V67" s="181"/>
+      <c r="W67" s="181"/>
+      <c r="X67" s="181"/>
+      <c r="Y67" s="181"/>
+      <c r="Z67" s="181"/>
+      <c r="AA67" s="181"/>
+      <c r="AB67" s="181"/>
+      <c r="AC67" s="181"/>
+      <c r="AD67" s="181"/>
+      <c r="AE67" s="181"/>
+      <c r="AF67" s="181"/>
+      <c r="AG67" s="181"/>
+      <c r="AH67" s="181"/>
+      <c r="AI67" s="181"/>
+      <c r="AJ67" s="181"/>
+      <c r="AK67" s="181"/>
+      <c r="AL67" s="182"/>
       <c r="AM67" s="2"/>
       <c r="AN67" s="2"/>
     </row>
@@ -14546,46 +14554,46 @@
         <v>F8</v>
       </c>
       <c r="D68" s="39"/>
-      <c r="E68" s="171"/>
+      <c r="E68" s="173"/>
       <c r="F68" s="57" t="str">
         <f t="shared" si="4"/>
         <v>R0.30 or R0.62</v>
       </c>
-      <c r="G68" s="179" t="str">
+      <c r="G68" s="180" t="str">
         <f t="shared" si="5"/>
         <v>R0.30 or R0.62</v>
       </c>
-      <c r="H68" s="180"/>
-      <c r="I68" s="180"/>
-      <c r="J68" s="180"/>
-      <c r="K68" s="180"/>
-      <c r="L68" s="180"/>
-      <c r="M68" s="180"/>
-      <c r="N68" s="180"/>
-      <c r="O68" s="180"/>
-      <c r="P68" s="180"/>
-      <c r="Q68" s="180"/>
-      <c r="R68" s="180"/>
-      <c r="S68" s="180"/>
-      <c r="T68" s="180"/>
-      <c r="U68" s="180"/>
-      <c r="V68" s="180"/>
-      <c r="W68" s="180"/>
-      <c r="X68" s="180"/>
-      <c r="Y68" s="180"/>
-      <c r="Z68" s="180"/>
-      <c r="AA68" s="180"/>
-      <c r="AB68" s="180"/>
-      <c r="AC68" s="180"/>
-      <c r="AD68" s="180"/>
-      <c r="AE68" s="180"/>
-      <c r="AF68" s="180"/>
-      <c r="AG68" s="180"/>
-      <c r="AH68" s="180"/>
-      <c r="AI68" s="180"/>
-      <c r="AJ68" s="180"/>
-      <c r="AK68" s="180"/>
-      <c r="AL68" s="181"/>
+      <c r="H68" s="181"/>
+      <c r="I68" s="181"/>
+      <c r="J68" s="181"/>
+      <c r="K68" s="181"/>
+      <c r="L68" s="181"/>
+      <c r="M68" s="181"/>
+      <c r="N68" s="181"/>
+      <c r="O68" s="181"/>
+      <c r="P68" s="181"/>
+      <c r="Q68" s="181"/>
+      <c r="R68" s="181"/>
+      <c r="S68" s="181"/>
+      <c r="T68" s="181"/>
+      <c r="U68" s="181"/>
+      <c r="V68" s="181"/>
+      <c r="W68" s="181"/>
+      <c r="X68" s="181"/>
+      <c r="Y68" s="181"/>
+      <c r="Z68" s="181"/>
+      <c r="AA68" s="181"/>
+      <c r="AB68" s="181"/>
+      <c r="AC68" s="181"/>
+      <c r="AD68" s="181"/>
+      <c r="AE68" s="181"/>
+      <c r="AF68" s="181"/>
+      <c r="AG68" s="181"/>
+      <c r="AH68" s="181"/>
+      <c r="AI68" s="181"/>
+      <c r="AJ68" s="181"/>
+      <c r="AK68" s="181"/>
+      <c r="AL68" s="182"/>
       <c r="AM68" s="2"/>
       <c r="AN68" s="2"/>
     </row>
@@ -14599,46 +14607,46 @@
         <v>FC</v>
       </c>
       <c r="D69" s="52"/>
-      <c r="E69" s="172"/>
+      <c r="E69" s="174"/>
       <c r="F69" s="71" t="str">
         <f t="shared" si="4"/>
         <v>R0.31 or R0.63</v>
       </c>
-      <c r="G69" s="189" t="str">
+      <c r="G69" s="177" t="str">
         <f>F69</f>
         <v>R0.31 or R0.63</v>
       </c>
-      <c r="H69" s="190"/>
-      <c r="I69" s="190"/>
-      <c r="J69" s="190"/>
-      <c r="K69" s="190"/>
-      <c r="L69" s="190"/>
-      <c r="M69" s="190"/>
-      <c r="N69" s="190"/>
-      <c r="O69" s="190"/>
-      <c r="P69" s="190"/>
-      <c r="Q69" s="190"/>
-      <c r="R69" s="190"/>
-      <c r="S69" s="190"/>
-      <c r="T69" s="190"/>
-      <c r="U69" s="190"/>
-      <c r="V69" s="190"/>
-      <c r="W69" s="190"/>
-      <c r="X69" s="190"/>
-      <c r="Y69" s="190"/>
-      <c r="Z69" s="190"/>
-      <c r="AA69" s="190"/>
-      <c r="AB69" s="190"/>
-      <c r="AC69" s="190"/>
-      <c r="AD69" s="190"/>
-      <c r="AE69" s="190"/>
-      <c r="AF69" s="190"/>
-      <c r="AG69" s="190"/>
-      <c r="AH69" s="190"/>
-      <c r="AI69" s="190"/>
-      <c r="AJ69" s="190"/>
-      <c r="AK69" s="190"/>
-      <c r="AL69" s="191"/>
+      <c r="H69" s="178"/>
+      <c r="I69" s="178"/>
+      <c r="J69" s="178"/>
+      <c r="K69" s="178"/>
+      <c r="L69" s="178"/>
+      <c r="M69" s="178"/>
+      <c r="N69" s="178"/>
+      <c r="O69" s="178"/>
+      <c r="P69" s="178"/>
+      <c r="Q69" s="178"/>
+      <c r="R69" s="178"/>
+      <c r="S69" s="178"/>
+      <c r="T69" s="178"/>
+      <c r="U69" s="178"/>
+      <c r="V69" s="178"/>
+      <c r="W69" s="178"/>
+      <c r="X69" s="178"/>
+      <c r="Y69" s="178"/>
+      <c r="Z69" s="178"/>
+      <c r="AA69" s="178"/>
+      <c r="AB69" s="178"/>
+      <c r="AC69" s="178"/>
+      <c r="AD69" s="178"/>
+      <c r="AE69" s="178"/>
+      <c r="AF69" s="178"/>
+      <c r="AG69" s="178"/>
+      <c r="AH69" s="178"/>
+      <c r="AI69" s="178"/>
+      <c r="AJ69" s="178"/>
+      <c r="AK69" s="178"/>
+      <c r="AL69" s="179"/>
       <c r="AM69" s="2"/>
       <c r="AN69" s="2"/>
     </row>
@@ -14668,6 +14676,78 @@
     </row>
   </sheetData>
   <mergeCells count="88">
+    <mergeCell ref="X7:Z7"/>
+    <mergeCell ref="AB7:AD7"/>
+    <mergeCell ref="E38:E69"/>
+    <mergeCell ref="AI6:AK6"/>
+    <mergeCell ref="E6:E13"/>
+    <mergeCell ref="AF7:AH7"/>
+    <mergeCell ref="AJ7:AL7"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="AJ9:AL9"/>
+    <mergeCell ref="AF9:AH9"/>
+    <mergeCell ref="AB9:AD9"/>
+    <mergeCell ref="X9:Z9"/>
+    <mergeCell ref="T9:V9"/>
+    <mergeCell ref="AA6:AD6"/>
+    <mergeCell ref="AG30:AH30"/>
+    <mergeCell ref="AC30:AD30"/>
+    <mergeCell ref="Y30:Z30"/>
+    <mergeCell ref="G45:AL45"/>
+    <mergeCell ref="G15:AL15"/>
+    <mergeCell ref="G16:AL16"/>
+    <mergeCell ref="G40:AL40"/>
+    <mergeCell ref="G41:AL41"/>
+    <mergeCell ref="G42:AL42"/>
+    <mergeCell ref="G43:AL43"/>
+    <mergeCell ref="G44:AL44"/>
+    <mergeCell ref="L31:N31"/>
+    <mergeCell ref="P31:R31"/>
+    <mergeCell ref="T31:V31"/>
+    <mergeCell ref="X31:Z31"/>
+    <mergeCell ref="AB31:AD31"/>
+    <mergeCell ref="I30:V30"/>
+    <mergeCell ref="D2:AL2"/>
+    <mergeCell ref="G38:AL38"/>
+    <mergeCell ref="G39:AL39"/>
+    <mergeCell ref="G26:AL26"/>
+    <mergeCell ref="G27:AL27"/>
+    <mergeCell ref="G28:AL28"/>
+    <mergeCell ref="G29:AL29"/>
+    <mergeCell ref="AE18:AL18"/>
+    <mergeCell ref="G19:AL19"/>
+    <mergeCell ref="G20:AL20"/>
+    <mergeCell ref="AJ37:AL37"/>
+    <mergeCell ref="G22:AL22"/>
+    <mergeCell ref="G23:AL23"/>
+    <mergeCell ref="AK30:AL30"/>
+    <mergeCell ref="AF8:AH8"/>
+    <mergeCell ref="AJ8:AL8"/>
+    <mergeCell ref="G57:AL57"/>
+    <mergeCell ref="G46:AL46"/>
+    <mergeCell ref="G47:AL47"/>
+    <mergeCell ref="G48:AL48"/>
+    <mergeCell ref="G49:AL49"/>
+    <mergeCell ref="G50:AL50"/>
+    <mergeCell ref="G51:AL51"/>
+    <mergeCell ref="G52:AL52"/>
+    <mergeCell ref="G53:AL53"/>
+    <mergeCell ref="G54:AL54"/>
+    <mergeCell ref="G55:AL55"/>
+    <mergeCell ref="G56:AL56"/>
+    <mergeCell ref="G69:AL69"/>
+    <mergeCell ref="G58:AL58"/>
+    <mergeCell ref="G59:AL59"/>
+    <mergeCell ref="G60:AL60"/>
+    <mergeCell ref="G61:AL61"/>
+    <mergeCell ref="G62:AL62"/>
+    <mergeCell ref="G63:AL63"/>
+    <mergeCell ref="G64:AL64"/>
+    <mergeCell ref="G65:AL65"/>
+    <mergeCell ref="G66:AL66"/>
+    <mergeCell ref="G67:AL67"/>
+    <mergeCell ref="G68:AL68"/>
     <mergeCell ref="AE6:AG6"/>
     <mergeCell ref="H31:J31"/>
     <mergeCell ref="AF31:AH31"/>
@@ -14684,78 +14764,6 @@
     <mergeCell ref="AB8:AD8"/>
     <mergeCell ref="L7:N7"/>
     <mergeCell ref="P7:R7"/>
-    <mergeCell ref="G69:AL69"/>
-    <mergeCell ref="G58:AL58"/>
-    <mergeCell ref="G59:AL59"/>
-    <mergeCell ref="G60:AL60"/>
-    <mergeCell ref="G61:AL61"/>
-    <mergeCell ref="G62:AL62"/>
-    <mergeCell ref="G63:AL63"/>
-    <mergeCell ref="G64:AL64"/>
-    <mergeCell ref="G65:AL65"/>
-    <mergeCell ref="G66:AL66"/>
-    <mergeCell ref="G67:AL67"/>
-    <mergeCell ref="G68:AL68"/>
-    <mergeCell ref="G57:AL57"/>
-    <mergeCell ref="G46:AL46"/>
-    <mergeCell ref="G47:AL47"/>
-    <mergeCell ref="G48:AL48"/>
-    <mergeCell ref="G49:AL49"/>
-    <mergeCell ref="G50:AL50"/>
-    <mergeCell ref="G51:AL51"/>
-    <mergeCell ref="G52:AL52"/>
-    <mergeCell ref="G53:AL53"/>
-    <mergeCell ref="G54:AL54"/>
-    <mergeCell ref="G55:AL55"/>
-    <mergeCell ref="G56:AL56"/>
-    <mergeCell ref="D2:AL2"/>
-    <mergeCell ref="G38:AL38"/>
-    <mergeCell ref="G39:AL39"/>
-    <mergeCell ref="G26:AL26"/>
-    <mergeCell ref="G27:AL27"/>
-    <mergeCell ref="G28:AL28"/>
-    <mergeCell ref="G29:AL29"/>
-    <mergeCell ref="AE18:AL18"/>
-    <mergeCell ref="G19:AL19"/>
-    <mergeCell ref="G20:AL20"/>
-    <mergeCell ref="AJ37:AL37"/>
-    <mergeCell ref="G22:AL22"/>
-    <mergeCell ref="G23:AL23"/>
-    <mergeCell ref="AK30:AL30"/>
-    <mergeCell ref="AF8:AH8"/>
-    <mergeCell ref="AJ8:AL8"/>
-    <mergeCell ref="AC30:AD30"/>
-    <mergeCell ref="Y30:Z30"/>
-    <mergeCell ref="G45:AL45"/>
-    <mergeCell ref="G15:AL15"/>
-    <mergeCell ref="G16:AL16"/>
-    <mergeCell ref="G40:AL40"/>
-    <mergeCell ref="G41:AL41"/>
-    <mergeCell ref="G42:AL42"/>
-    <mergeCell ref="G43:AL43"/>
-    <mergeCell ref="G44:AL44"/>
-    <mergeCell ref="L31:N31"/>
-    <mergeCell ref="P31:R31"/>
-    <mergeCell ref="T31:V31"/>
-    <mergeCell ref="X31:Z31"/>
-    <mergeCell ref="AB31:AD31"/>
-    <mergeCell ref="I30:V30"/>
-    <mergeCell ref="X7:Z7"/>
-    <mergeCell ref="AB7:AD7"/>
-    <mergeCell ref="E38:E69"/>
-    <mergeCell ref="AI6:AK6"/>
-    <mergeCell ref="E6:E13"/>
-    <mergeCell ref="AF7:AH7"/>
-    <mergeCell ref="AJ7:AL7"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="AJ9:AL9"/>
-    <mergeCell ref="AF9:AH9"/>
-    <mergeCell ref="AB9:AD9"/>
-    <mergeCell ref="X9:Z9"/>
-    <mergeCell ref="T9:V9"/>
-    <mergeCell ref="AA6:AD6"/>
-    <mergeCell ref="AG30:AH30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>